<commit_message>
Basic program flow for uploading simulation results
</commit_message>
<xml_diff>
--- a/Temporary Region Swings.xlsx
+++ b/Temporary Region Swings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E13953-C95F-4C40-BD1C-77A30A9B1ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDFFB6E-43F0-4B8C-B800-38A2D500BDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1185" windowWidth="17700" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19335" yWindow="6225" windowWidth="9465" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="1" r:id="rId1"/>
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,22 +639,22 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>54</v>
+        <v>55.5</v>
       </c>
       <c r="C6">
         <v>55.5</v>
       </c>
       <c r="D6">
-        <v>56.5</v>
+        <v>58</v>
       </c>
       <c r="E6">
-        <v>48.5</v>
+        <v>51.5</v>
       </c>
       <c r="F6">
-        <v>55</v>
+        <v>53.5</v>
       </c>
       <c r="G6">
-        <v>48.5</v>
+        <v>55.5</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -662,22 +662,22 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>53</v>
+        <v>53.5</v>
       </c>
       <c r="C7">
         <v>53.5</v>
       </c>
       <c r="D7">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F7">
-        <v>55</v>
+        <v>53.5</v>
       </c>
       <c r="G7">
-        <v>54.5</v>
+        <v>57.5</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -688,19 +688,19 @@
         <v>54</v>
       </c>
       <c r="C8">
-        <v>53.5</v>
+        <v>55.5</v>
       </c>
       <c r="D8">
-        <v>56</v>
+        <v>56.5</v>
       </c>
       <c r="E8">
-        <v>47.5</v>
+        <v>48.5</v>
       </c>
       <c r="F8">
-        <v>54.5</v>
+        <v>55</v>
       </c>
       <c r="G8">
-        <v>58.5</v>
+        <v>48.5</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -935,7 +935,7 @@
       </c>
       <c r="C19">
         <f t="shared" ref="C19:G19" si="1">(C6-C$2)-($B6-$B$2)</f>
-        <v>1.75</v>
+        <v>0.25</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
@@ -943,19 +943,19 @@
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>1.4099999999999966</v>
+        <v>2.9099999999999966</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>5.019999999999996</v>
+        <v>2.019999999999996</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>-7.740000000000002</v>
+        <v>-2.240000000000002</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" ref="H19:H21" si="2">F19*0.439183+G19*0.336042</f>
-        <v>-0.39626642000000256</v>
+        <v>0.13441557999999765</v>
       </c>
       <c r="J19">
         <v>1401874</v>
@@ -979,27 +979,27 @@
       </c>
       <c r="C20">
         <f t="shared" ref="C20:G20" si="3">(C7-C$2)-($B7-$B$2)</f>
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="D20">
         <f t="shared" si="3"/>
-        <v>-1.6700000000000017</v>
+        <v>-3.1700000000000017</v>
       </c>
       <c r="E20">
         <f t="shared" si="3"/>
-        <v>-1.0900000000000034</v>
+        <v>0.40999999999999659</v>
       </c>
       <c r="F20">
         <f t="shared" si="3"/>
-        <v>6.019999999999996</v>
+        <v>4.019999999999996</v>
       </c>
       <c r="G20">
         <f t="shared" si="3"/>
-        <v>-0.74000000000000199</v>
+        <v>1.759999999999998</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="2"/>
-        <v>2.3952105799999974</v>
+        <v>2.3569495799999975</v>
       </c>
       <c r="J20">
         <f>J19/SUM($J19:$N19)</f>
@@ -1016,27 +1016,27 @@
       </c>
       <c r="C21">
         <f t="shared" ref="C21:G21" si="4">(C8-C$2)-($B8-$B$2)</f>
-        <v>-0.25</v>
+        <v>1.75</v>
       </c>
       <c r="D21">
         <f t="shared" si="4"/>
-        <v>-2.6700000000000017</v>
+        <v>-2.1700000000000017</v>
       </c>
       <c r="E21">
         <f t="shared" si="4"/>
-        <v>0.40999999999999659</v>
+        <v>1.4099999999999966</v>
       </c>
       <c r="F21">
         <f t="shared" si="4"/>
-        <v>4.519999999999996</v>
+        <v>5.019999999999996</v>
       </c>
       <c r="G21">
         <f t="shared" si="4"/>
-        <v>2.259999999999998</v>
+        <v>-7.740000000000002</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="2"/>
-        <v>2.7445620799999979</v>
+        <v>-0.39626642000000256</v>
       </c>
       <c r="L21">
         <f>(J19+K19)/SUM(J19:N19)</f>
@@ -1061,11 +1061,11 @@
       </c>
       <c r="F22" s="2">
         <f>AVERAGE(F$18,F$18,F$18,F$18,F$18,F$18,F$19,F$20,F$21)+($H22-AVERAGE($H$18,$H$18,$H$18,$H$18,$H$18,$H$18,$H$19,$H$20,$H$21))</f>
-        <v>7.0000241203419886</v>
+        <v>6.7942916203419887</v>
       </c>
       <c r="G22" s="2">
         <f>AVERAGE(G$18,G$18,G$18,G$18,G$18,G$18,G$19,G$20,G$21)+($H22-AVERAGE($H$18,$H$18,$H$18,$H$18,$H$18,$H$18,$H$19,$H$20,$H$21))</f>
-        <v>-0.25997587965800939</v>
+        <v>-0.18793060188023114</v>
       </c>
       <c r="H22">
         <f>(H9-H$2)-($B9-$B$2)</f>
@@ -1090,11 +1090,11 @@
       </c>
       <c r="F23" s="2">
         <f t="shared" ref="F23:G24" si="7">AVERAGE(F$18,F$18,F$18,F$18,F$18,F$18,F$19,F$20,F$21)+($H23-AVERAGE($H$18,$H$18,$H$18,$H$18,$H$18,$H$18,$H$19,$H$20,$H$21))</f>
-        <v>5.3590241203419833</v>
+        <v>5.1532916203419834</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="7"/>
-        <v>-1.9009758796580147</v>
+        <v>-1.8289306018802365</v>
       </c>
       <c r="H23">
         <f>(H10-H$2)-($B10-$B$2)</f>
@@ -1119,11 +1119,11 @@
       </c>
       <c r="F24" s="2">
         <f t="shared" si="7"/>
-        <v>3.6970241203419771</v>
+        <v>3.4912916203419773</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" si="7"/>
-        <v>-3.5629758796580209</v>
+        <v>-3.4909306018802426</v>
       </c>
       <c r="H24">
         <f>(H11-H$2)-($B11-$B$2)</f>
@@ -1253,19 +1253,19 @@
       </c>
       <c r="D30">
         <f t="shared" ref="D30:G30" si="13">AVERAGE(D18,D18,D18,D18,D18,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28)</f>
-        <v>-1.6942406930940948</v>
+        <v>-1.7567406930940948</v>
       </c>
       <c r="E30">
         <f t="shared" si="13"/>
-        <v>3.177271350043521</v>
+        <v>3.427271350043521</v>
       </c>
       <c r="F30">
         <f t="shared" si="13"/>
-        <v>5.8515898809492466</v>
+        <v>5.5317650371992455</v>
       </c>
       <c r="G30">
         <f t="shared" si="13"/>
-        <v>-2.2480966513575584</v>
+        <v>-2.3595881617742256</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -1275,19 +1275,19 @@
       </c>
       <c r="D31">
         <f>53.14+D30</f>
-        <v>51.445759306905906</v>
+        <v>51.383259306905906</v>
       </c>
       <c r="E31">
         <f>41.56+E30</f>
-        <v>44.737271350043521</v>
+        <v>44.987271350043521</v>
       </c>
       <c r="F31">
         <f>44.45+F30</f>
-        <v>50.301589880949251</v>
+        <v>49.981765037199246</v>
       </c>
       <c r="G31">
         <f>50.71+G30</f>
-        <v>48.461903348642444</v>
+        <v>48.350411838225774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Also update the regional swings
</commit_message>
<xml_diff>
--- a/Temporary Region Swings.xlsx
+++ b/Temporary Region Swings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git repositories\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDFFB6E-43F0-4B8C-B800-38A2D500BDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AA7951-48C1-4493-A309-6DD0C8BAC177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19335" yWindow="6225" windowWidth="9465" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14520" yWindow="540" windowWidth="21855" windowHeight="14835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="1" r:id="rId1"/>
@@ -480,7 +480,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,22 +639,22 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>55.5</v>
+        <v>56.5</v>
       </c>
       <c r="C6">
         <v>55.5</v>
       </c>
       <c r="D6">
-        <v>58</v>
+        <v>58.5</v>
       </c>
       <c r="E6">
-        <v>51.5</v>
+        <v>54.5</v>
       </c>
       <c r="F6">
-        <v>53.5</v>
+        <v>50.5</v>
       </c>
       <c r="G6">
-        <v>55.5</v>
+        <v>64.5</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -662,22 +662,22 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>53.5</v>
+        <v>55.5</v>
       </c>
       <c r="C7">
-        <v>53.5</v>
+        <v>55.5</v>
       </c>
       <c r="D7">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E7">
-        <v>47</v>
+        <v>51.5</v>
       </c>
       <c r="F7">
         <v>53.5</v>
       </c>
       <c r="G7">
-        <v>57.5</v>
+        <v>55.5</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -685,22 +685,22 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>54</v>
+        <v>53.5</v>
       </c>
       <c r="C8">
-        <v>55.5</v>
+        <v>53.5</v>
       </c>
       <c r="D8">
-        <v>56.5</v>
+        <v>55</v>
       </c>
       <c r="E8">
-        <v>48.5</v>
+        <v>47</v>
       </c>
       <c r="F8">
-        <v>55</v>
+        <v>53.5</v>
       </c>
       <c r="G8">
-        <v>48.5</v>
+        <v>57.5</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -935,27 +935,27 @@
       </c>
       <c r="C19">
         <f t="shared" ref="C19:G19" si="1">(C6-C$2)-($B6-$B$2)</f>
-        <v>0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>-2.1700000000000017</v>
+        <v>-2.6700000000000017</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>2.9099999999999966</v>
+        <v>4.9099999999999966</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>2.019999999999996</v>
+        <v>-1.980000000000004</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>-2.240000000000002</v>
+        <v>5.759999999999998</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" ref="H19:H21" si="2">F19*0.439183+G19*0.336042</f>
-        <v>0.13441557999999765</v>
+        <v>1.0660195799999976</v>
       </c>
       <c r="J19">
         <v>1401874</v>
@@ -983,23 +983,23 @@
       </c>
       <c r="D20">
         <f t="shared" si="3"/>
-        <v>-3.1700000000000017</v>
+        <v>-2.1700000000000017</v>
       </c>
       <c r="E20">
         <f t="shared" si="3"/>
-        <v>0.40999999999999659</v>
+        <v>2.9099999999999966</v>
       </c>
       <c r="F20">
         <f t="shared" si="3"/>
-        <v>4.019999999999996</v>
+        <v>2.019999999999996</v>
       </c>
       <c r="G20">
         <f t="shared" si="3"/>
-        <v>1.759999999999998</v>
+        <v>-2.240000000000002</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="2"/>
-        <v>2.3569495799999975</v>
+        <v>0.13441557999999765</v>
       </c>
       <c r="J20">
         <f>J19/SUM($J19:$N19)</f>
@@ -1016,27 +1016,27 @@
       </c>
       <c r="C21">
         <f t="shared" ref="C21:G21" si="4">(C8-C$2)-($B8-$B$2)</f>
-        <v>1.75</v>
+        <v>0.25</v>
       </c>
       <c r="D21">
         <f t="shared" si="4"/>
-        <v>-2.1700000000000017</v>
+        <v>-3.1700000000000017</v>
       </c>
       <c r="E21">
         <f t="shared" si="4"/>
-        <v>1.4099999999999966</v>
+        <v>0.40999999999999659</v>
       </c>
       <c r="F21">
         <f t="shared" si="4"/>
-        <v>5.019999999999996</v>
+        <v>4.019999999999996</v>
       </c>
       <c r="G21">
         <f t="shared" si="4"/>
-        <v>-7.740000000000002</v>
+        <v>1.759999999999998</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="2"/>
-        <v>-0.39626642000000256</v>
+        <v>2.3569495799999975</v>
       </c>
       <c r="L21">
         <f>(J19+K19)/SUM(J19:N19)</f>
@@ -1061,11 +1061,11 @@
       </c>
       <c r="F22" s="2">
         <f>AVERAGE(F$18,F$18,F$18,F$18,F$18,F$18,F$19,F$20,F$21)+($H22-AVERAGE($H$18,$H$18,$H$18,$H$18,$H$18,$H$18,$H$19,$H$20,$H$21))</f>
-        <v>6.7942916203419887</v>
+        <v>5.8540376203419893</v>
       </c>
       <c r="G22" s="2">
         <f>AVERAGE(G$18,G$18,G$18,G$18,G$18,G$18,G$19,G$20,G$21)+($H22-AVERAGE($H$18,$H$18,$H$18,$H$18,$H$18,$H$18,$H$19,$H$20,$H$21))</f>
-        <v>-0.18793060188023114</v>
+        <v>1.1495931758975471</v>
       </c>
       <c r="H22">
         <f>(H9-H$2)-($B9-$B$2)</f>
@@ -1090,11 +1090,11 @@
       </c>
       <c r="F23" s="2">
         <f t="shared" ref="F23:G24" si="7">AVERAGE(F$18,F$18,F$18,F$18,F$18,F$18,F$19,F$20,F$21)+($H23-AVERAGE($H$18,$H$18,$H$18,$H$18,$H$18,$H$18,$H$19,$H$20,$H$21))</f>
-        <v>5.1532916203419834</v>
+        <v>4.2130376203419839</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="7"/>
-        <v>-1.8289306018802365</v>
+        <v>-0.49140682410245862</v>
       </c>
       <c r="H23">
         <f>(H10-H$2)-($B10-$B$2)</f>
@@ -1119,11 +1119,11 @@
       </c>
       <c r="F24" s="2">
         <f t="shared" si="7"/>
-        <v>3.4912916203419773</v>
+        <v>2.5510376203419778</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" si="7"/>
-        <v>-3.4909306018802426</v>
+        <v>-2.1534068241024649</v>
       </c>
       <c r="H24">
         <f>(H11-H$2)-($B11-$B$2)</f>
@@ -1249,45 +1249,45 @@
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C30">
         <f>AVERAGE(C18,C18,C18,C18,C18,C18,C19,C20,C21,C22,C23,C24,C25,C26,C27,C28)</f>
-        <v>-1.1662021100119881</v>
+        <v>-1.3224521100119881</v>
       </c>
       <c r="D30">
         <f t="shared" ref="D30:G30" si="13">AVERAGE(D18,D18,D18,D18,D18,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28)</f>
-        <v>-1.7567406930940948</v>
+        <v>-1.7879906930940948</v>
       </c>
       <c r="E30">
         <f t="shared" si="13"/>
-        <v>3.427271350043521</v>
+        <v>3.646021350043521</v>
       </c>
       <c r="F30">
         <f t="shared" si="13"/>
-        <v>5.5317650371992455</v>
+        <v>4.9179674121992463</v>
       </c>
       <c r="G30">
         <f t="shared" si="13"/>
-        <v>-2.3595881617742256</v>
+        <v>-1.265052453440892</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C31">
         <f>48.22+C30</f>
-        <v>47.053797889988012</v>
+        <v>46.897547889988012</v>
       </c>
       <c r="D31">
         <f>53.14+D30</f>
-        <v>51.383259306905906</v>
+        <v>51.352009306905906</v>
       </c>
       <c r="E31">
         <f>41.56+E30</f>
-        <v>44.987271350043521</v>
+        <v>45.206021350043521</v>
       </c>
       <c r="F31">
         <f>44.45+F30</f>
-        <v>49.981765037199246</v>
+        <v>49.367967412199249</v>
       </c>
       <c r="G31">
         <f>50.71+G30</f>
-        <v>48.350411838225774</v>
+        <v>49.444947546559106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Vic file with substitute past results and non-classic pref flows
</commit_message>
<xml_diff>
--- a/Temporary Region Swings.xlsx
+++ b/Temporary Region Swings.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git repositories\Polling Analyser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AA7951-48C1-4493-A309-6DD0C8BAC177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F91AF5B-74A4-4D58-A1FE-8CF6B9F3EF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="540" windowWidth="21855" windowHeight="14835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="900" windowWidth="24255" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="1" r:id="rId1"/>
     <sheet name="Archives" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -477,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,19 +620,19 @@
         <v>53</v>
       </c>
       <c r="C5">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D5">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E5">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F5">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G5">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -886,28 +887,28 @@
         <v>7</v>
       </c>
       <c r="C18">
-        <f>(C5-C$2)-($B5-$B$2)</f>
-        <v>-0.75</v>
+        <f t="shared" ref="C18:G21" si="0">(C5-C$2)-($B5-$B$2)</f>
+        <v>0.25</v>
       </c>
       <c r="D18">
-        <f t="shared" ref="D18:G18" si="0">(D5-D$2)-($B5-$B$2)</f>
-        <v>0.32999999999999829</v>
+        <f t="shared" si="0"/>
+        <v>-1.6700000000000017</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>-1.0900000000000034</v>
+        <v>-9.0000000000003411E-2</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>5.019999999999996</v>
+        <v>6.019999999999996</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>-2.240000000000002</v>
+        <v>-0.24000000000000199</v>
       </c>
       <c r="H18" s="2">
         <f>F18*0.439183+G18*0.336042</f>
-        <v>1.4519645799999976</v>
+        <v>2.5632315799999974</v>
       </c>
       <c r="J18">
         <v>44.45</v>
@@ -934,27 +935,27 @@
         <v>8</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:G19" si="1">(C6-C$2)-($B6-$B$2)</f>
+        <f t="shared" si="0"/>
         <v>-0.75</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-2.6700000000000017</v>
       </c>
       <c r="E19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.9099999999999966</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-1.980000000000004</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5.759999999999998</v>
       </c>
       <c r="H19" s="2">
-        <f t="shared" ref="H19:H21" si="2">F19*0.439183+G19*0.336042</f>
+        <f>F19*0.439183+G19*0.336042</f>
         <v>1.0660195799999976</v>
       </c>
       <c r="J19">
@@ -978,27 +979,27 @@
         <v>9</v>
       </c>
       <c r="C20">
-        <f t="shared" ref="C20:G20" si="3">(C7-C$2)-($B7-$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="D20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>-2.1700000000000017</v>
       </c>
       <c r="E20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>2.9099999999999966</v>
       </c>
       <c r="F20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>2.019999999999996</v>
       </c>
       <c r="G20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>-2.240000000000002</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" si="2"/>
+        <f>F20*0.439183+G20*0.336042</f>
         <v>0.13441557999999765</v>
       </c>
       <c r="J20">
@@ -1015,27 +1016,27 @@
         <v>10</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:G21" si="4">(C8-C$2)-($B8-$B$2)</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="D21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>-3.1700000000000017</v>
       </c>
       <c r="E21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.40999999999999659</v>
       </c>
       <c r="F21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>4.019999999999996</v>
       </c>
       <c r="G21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1.759999999999998</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" si="2"/>
+        <f>F21*0.439183+G21*0.336042</f>
         <v>2.3569495799999975</v>
       </c>
       <c r="L21">
@@ -1048,24 +1049,24 @@
         <v>11</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:E22" si="5">(C9-C$2)-($B9-$B$2)</f>
+        <f t="shared" ref="C22:E26" si="1">(C9-C$2)-($B9-$B$2)</f>
         <v>-1.5769999999999982</v>
       </c>
       <c r="D22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>-0.37100000000000222</v>
       </c>
       <c r="E22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>3.2929999999999993</v>
       </c>
       <c r="F22" s="2">
-        <f>AVERAGE(F$18,F$18,F$18,F$18,F$18,F$18,F$19,F$20,F$21)+($H22-AVERAGE($H$18,$H$18,$H$18,$H$18,$H$18,$H$18,$H$19,$H$20,$H$21))</f>
-        <v>5.8540376203419893</v>
+        <f t="shared" ref="F22:G24" si="2">AVERAGE(F$18,F$18,F$18,F$18,F$18,F$18,F$19,F$20,F$21)+($H22-AVERAGE($H$18,$H$18,$H$18,$H$18,$H$18,$H$18,$H$19,$H$20,$H$21))</f>
+        <v>5.7798596203419894</v>
       </c>
       <c r="G22" s="2">
-        <f>AVERAGE(G$18,G$18,G$18,G$18,G$18,G$18,G$19,G$20,G$21)+($H22-AVERAGE($H$18,$H$18,$H$18,$H$18,$H$18,$H$18,$H$19,$H$20,$H$21))</f>
-        <v>1.1495931758975471</v>
+        <f t="shared" si="2"/>
+        <v>1.7420818425642131</v>
       </c>
       <c r="H22">
         <f>(H9-H$2)-($B9-$B$2)</f>
@@ -1077,24 +1078,24 @@
         <v>19</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:E23" si="6">(C10-C$2)-($B10-$B$2)</f>
+        <f t="shared" si="1"/>
         <v>-0.28699999999999193</v>
       </c>
       <c r="D23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>-3.2010000000000005</v>
       </c>
       <c r="E23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>6.159000000000006</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" ref="F23:G24" si="7">AVERAGE(F$18,F$18,F$18,F$18,F$18,F$18,F$19,F$20,F$21)+($H23-AVERAGE($H$18,$H$18,$H$18,$H$18,$H$18,$H$18,$H$19,$H$20,$H$21))</f>
-        <v>4.2130376203419839</v>
+        <f t="shared" si="2"/>
+        <v>4.1388596203419841</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="7"/>
-        <v>-0.49140682410245862</v>
+        <f t="shared" si="2"/>
+        <v>0.10108184256420766</v>
       </c>
       <c r="H23">
         <f>(H10-H$2)-($B10-$B$2)</f>
@@ -1106,24 +1107,24 @@
         <v>20</v>
       </c>
       <c r="C24">
-        <f t="shared" ref="C24:E24" si="8">(C11-C$2)-($B11-$B$2)</f>
+        <f t="shared" si="1"/>
         <v>-1.460000000000008</v>
       </c>
       <c r="D24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>-2.0370000000000061</v>
       </c>
       <c r="E24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>6.9559999999999889</v>
       </c>
       <c r="F24" s="2">
-        <f t="shared" si="7"/>
-        <v>2.5510376203419778</v>
+        <f t="shared" si="2"/>
+        <v>2.4768596203419775</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="7"/>
-        <v>-2.1534068241024649</v>
+        <f t="shared" si="2"/>
+        <v>-1.5609181574357984</v>
       </c>
       <c r="H24">
         <f>(H11-H$2)-($B11-$B$2)</f>
@@ -1135,23 +1136,23 @@
         <v>31</v>
       </c>
       <c r="C25">
-        <f>(C12-C$2)-($B12-$B$2)</f>
+        <f t="shared" si="1"/>
         <v>-6.2016129032258007</v>
       </c>
       <c r="D25">
-        <f t="shared" ref="D25:G25" si="9">(D12-D$2)-($B12-$B$2)</f>
+        <f t="shared" si="1"/>
         <v>-7.861850594227505</v>
       </c>
       <c r="E25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>15.935394646533972</v>
       </c>
       <c r="F25">
-        <f t="shared" si="9"/>
+        <f>(F12-F$2)-($B12-$B$2)</f>
         <v>7.2458064516128999</v>
       </c>
       <c r="G25">
-        <f t="shared" si="9"/>
+        <f>(G12-G$2)-($B12-$B$2)</f>
         <v>-4.916733013040492</v>
       </c>
       <c r="H25" s="2">
@@ -1164,27 +1165,27 @@
         <v>32</v>
       </c>
       <c r="C26">
-        <f t="shared" ref="C26:G26" si="10">(C13-C$2)-($B13-$B$2)</f>
+        <f t="shared" si="1"/>
         <v>-0.86111111111111427</v>
       </c>
       <c r="D26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="1"/>
         <v>-5.781111111111116</v>
       </c>
       <c r="E26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="1"/>
         <v>10.971302681992327</v>
       </c>
       <c r="F26">
-        <f t="shared" si="10"/>
+        <f>(F13-F$2)-($B13-$B$2)</f>
         <v>5.5970609318996338</v>
       </c>
       <c r="G26">
-        <f t="shared" si="10"/>
+        <f>(G13-G$2)-($B13-$B$2)</f>
         <v>-2.8016605616605688</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" ref="H26:H28" si="11">F26*0.439183+G26*0.336042</f>
+        <f>F26*0.439183+G26*0.336042</f>
         <v>1.516658392792936</v>
       </c>
     </row>
@@ -1193,27 +1194,27 @@
         <v>33</v>
       </c>
       <c r="C27">
-        <f t="shared" ref="C27:G28" si="12">(C14-C$2)-($B14-$B$2)</f>
+        <f t="shared" ref="C27:G28" si="3">(C14-C$2)-($B14-$B$2)</f>
         <v>-2.9758064486021496</v>
       </c>
       <c r="D27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="3"/>
         <v>-2.0390231038297841</v>
       </c>
       <c r="E27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="3"/>
         <v>5.8347311858064472</v>
       </c>
       <c r="F27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="3"/>
         <v>4.5233173217021232</v>
       </c>
       <c r="G27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="3"/>
         <v>-1.164731179784944</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" si="11"/>
+        <f>F27*0.439183+G27*0.336042</f>
         <v>1.5951654761798113</v>
       </c>
     </row>
@@ -1222,72 +1223,88 @@
         <v>34</v>
       </c>
       <c r="C28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="3"/>
         <v>-3.0467032972527477</v>
       </c>
       <c r="D28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="3"/>
         <v>-1.2868662803370867</v>
       </c>
       <c r="E28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="3"/>
         <v>7.4969130863636266</v>
       </c>
       <c r="F28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="3"/>
         <v>14.523181028947363</v>
       </c>
       <c r="G28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="3"/>
         <v>-1.7024940282608725</v>
       </c>
       <c r="H28" s="2">
-        <f t="shared" si="11"/>
+        <f>F28*0.439183+G28*0.336042</f>
         <v>5.8062247155913491</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C30">
         <f>AVERAGE(C18,C18,C18,C18,C18,C18,C19,C20,C21,C22,C23,C24,C25,C26,C27,C28)</f>
-        <v>-1.3224521100119881</v>
+        <v>-0.94745211001198815</v>
       </c>
       <c r="D30">
-        <f t="shared" ref="D30:G30" si="13">AVERAGE(D18,D18,D18,D18,D18,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28)</f>
-        <v>-1.7879906930940948</v>
+        <f>AVERAGE(D18,D18,D18,D18,D18,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28)</f>
+        <v>-2.5379906930940948</v>
       </c>
       <c r="E30">
-        <f t="shared" si="13"/>
-        <v>3.646021350043521</v>
+        <f>AVERAGE(E18,E18,E18,E18,E18,E18,E19,E20,E21,E22,E23,E24,E25,E26,E27,E28)</f>
+        <v>4.0210213500435206</v>
       </c>
       <c r="F30">
-        <f t="shared" si="13"/>
-        <v>4.9179674121992463</v>
+        <f>AVERAGE(F18,F18,F18,F18,F18,F18,F19,F20,F21,F22,F23,F24,F25,F26,F27,F28)</f>
+        <v>5.2790590371992456</v>
       </c>
       <c r="G30">
-        <f t="shared" si="13"/>
-        <v>-1.265052453440892</v>
+        <f>AVERAGE(G18,G18,G18,G18,G18,G18,G19,G20,G21,G22,G23,G24,G25,G26,G27,G28)</f>
+        <v>-0.40396082844089209</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C31">
         <f>48.22+C30</f>
-        <v>46.897547889988012</v>
+        <v>47.272547889988012</v>
       </c>
       <c r="D31">
         <f>53.14+D30</f>
-        <v>51.352009306905906</v>
+        <v>50.602009306905906</v>
       </c>
       <c r="E31">
         <f>41.56+E30</f>
-        <v>45.206021350043521</v>
+        <v>45.581021350043521</v>
       </c>
       <c r="F31">
         <f>44.45+F30</f>
-        <v>49.367967412199249</v>
+        <v>49.729059037199249</v>
       </c>
       <c r="G31">
         <f>50.71+G30</f>
-        <v>49.444947546559106</v>
+        <v>50.306039171559107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f>9.26*0.832</f>
+        <v>7.7043199999999992</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f>20.48*0.619</f>
+        <v>12.67712</v>
+      </c>
+      <c r="B39">
+        <f>(A39-A38)/(20.48-9.26)</f>
+        <v>0.4432085561497327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fully update for new ResolvePM poll
</commit_message>
<xml_diff>
--- a/Temporary Region Swings.xlsx
+++ b/Temporary Region Swings.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F91AF5B-74A4-4D58-A1FE-8CF6B9F3EF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54418CA0-BBB6-423A-AD9C-57A0F473CC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="900" windowWidth="24255" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1605" yWindow="4965" windowWidth="24255" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="1" r:id="rId1"/>
     <sheet name="Archives" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -481,7 +480,7 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,26 +563,26 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J3">
+        <v>33</v>
+      </c>
+      <c r="K3">
         <v>35</v>
       </c>
-      <c r="K3">
-        <v>36</v>
-      </c>
       <c r="L3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>15</v>
+      </c>
+      <c r="O3">
         <v>5</v>
-      </c>
-      <c r="N3">
-        <v>9</v>
-      </c>
-      <c r="O3">
-        <v>3</v>
       </c>
       <c r="P3">
         <f>K3+L3*0.822+M3*0.348+(N3+O3)*(0.507)</f>
-        <v>53.688000000000002</v>
+        <v>54.055999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -709,19 +708,19 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>49.183999999999997</v>
+        <v>53.704999999999998</v>
       </c>
       <c r="C9">
-        <v>47.356999999999999</v>
+        <v>52.332000000000001</v>
       </c>
       <c r="D9">
-        <v>53.482999999999997</v>
+        <v>58.515999999999998</v>
       </c>
       <c r="E9">
-        <v>45.567</v>
+        <v>48.938000000000002</v>
       </c>
       <c r="H9">
-        <v>53.688000000000002</v>
+        <v>54.055999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -729,19 +728,19 @@
         <v>19</v>
       </c>
       <c r="B10">
-        <v>51.183999999999997</v>
+        <v>49.183999999999997</v>
       </c>
       <c r="C10">
-        <v>50.647000000000006</v>
+        <v>47.356999999999999</v>
       </c>
       <c r="D10">
-        <v>52.652999999999999</v>
+        <v>53.482999999999997</v>
       </c>
       <c r="E10">
-        <v>50.433000000000007</v>
+        <v>45.567</v>
       </c>
       <c r="H10">
-        <v>54.046999999999997</v>
+        <v>53.688000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -749,19 +748,19 @@
         <v>20</v>
       </c>
       <c r="B11">
-        <v>48.724000000000004</v>
+        <v>51.183999999999997</v>
       </c>
       <c r="C11">
-        <v>47.013999999999996</v>
+        <v>50.647000000000006</v>
       </c>
       <c r="D11">
-        <v>51.356999999999999</v>
+        <v>52.652999999999999</v>
       </c>
       <c r="E11">
-        <v>48.769999999999996</v>
+        <v>50.433000000000007</v>
       </c>
       <c r="H11">
-        <v>49.924999999999997</v>
+        <v>54.046999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1050,27 +1049,27 @@
       </c>
       <c r="C22">
         <f t="shared" ref="C22:E26" si="1">(C9-C$2)-($B9-$B$2)</f>
-        <v>-1.5769999999999982</v>
+        <v>-1.1229999999999976</v>
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
-        <v>-0.37100000000000222</v>
+        <v>0.14099999999999824</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
-        <v>3.2929999999999993</v>
+        <v>2.1430000000000007</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" ref="F22:G24" si="2">AVERAGE(F$18,F$18,F$18,F$18,F$18,F$18,F$19,F$20,F$21)+($H22-AVERAGE($H$18,$H$18,$H$18,$H$18,$H$18,$H$18,$H$19,$H$20,$H$21))</f>
-        <v>5.7798596203419894</v>
+        <v>1.6268596203419832</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="2"/>
-        <v>1.7420818425642131</v>
+        <v>-2.410918157435793</v>
       </c>
       <c r="H22">
         <f>(H9-H$2)-($B9-$B$2)</f>
-        <v>3.4195012003419905</v>
+        <v>-0.73349879965801534</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -1079,27 +1078,27 @@
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>-0.28699999999999193</v>
+        <v>-1.5769999999999982</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>-3.2010000000000005</v>
+        <v>-0.37100000000000222</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
-        <v>6.159000000000006</v>
+        <v>3.2929999999999993</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="2"/>
-        <v>4.1388596203419841</v>
+        <v>5.7798596203419894</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="2"/>
-        <v>0.10108184256420766</v>
+        <v>1.7420818425642131</v>
       </c>
       <c r="H23">
         <f>(H10-H$2)-($B10-$B$2)</f>
-        <v>1.7785012003419851</v>
+        <v>3.4195012003419905</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -1108,27 +1107,27 @@
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>-1.460000000000008</v>
+        <v>-0.28699999999999193</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>-2.0370000000000061</v>
+        <v>-3.2010000000000005</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
-        <v>6.9559999999999889</v>
+        <v>6.159000000000006</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" si="2"/>
-        <v>2.4768596203419775</v>
+        <v>4.1388596203419841</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" si="2"/>
-        <v>-1.5609181574357984</v>
+        <v>0.10108184256420766</v>
       </c>
       <c r="H24">
         <f>(H11-H$2)-($B11-$B$2)</f>
-        <v>0.11650120034197897</v>
+        <v>1.7785012003419851</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -1250,45 +1249,45 @@
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C30">
         <f>AVERAGE(C18,C18,C18,C18,C18,C18,C19,C20,C21,C22,C23,C24,C25,C26,C27,C28)</f>
-        <v>-0.94745211001198815</v>
+        <v>-0.9263896100119875</v>
       </c>
       <c r="D30">
         <f>AVERAGE(D18,D18,D18,D18,D18,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28)</f>
-        <v>-2.5379906930940948</v>
+        <v>-2.4018656930940945</v>
       </c>
       <c r="E30">
         <f>AVERAGE(E18,E18,E18,E18,E18,E18,E19,E20,E21,E22,E23,E24,E25,E26,E27,E28)</f>
-        <v>4.0210213500435206</v>
+        <v>3.7202088500435218</v>
       </c>
       <c r="F30">
         <f>AVERAGE(F18,F18,F18,F18,F18,F18,F19,F20,F21,F22,F23,F24,F25,F26,F27,F28)</f>
-        <v>5.2790590371992456</v>
+        <v>5.225934037199246</v>
       </c>
       <c r="G30">
         <f>AVERAGE(G18,G18,G18,G18,G18,G18,G19,G20,G21,G22,G23,G24,G25,G26,G27,G28)</f>
-        <v>-0.40396082844089209</v>
+        <v>-0.45708582844089174</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C31">
         <f>48.22+C30</f>
-        <v>47.272547889988012</v>
+        <v>47.293610389988011</v>
       </c>
       <c r="D31">
         <f>53.14+D30</f>
-        <v>50.602009306905906</v>
+        <v>50.738134306905906</v>
       </c>
       <c r="E31">
         <f>41.56+E30</f>
-        <v>45.581021350043521</v>
+        <v>45.280208850043522</v>
       </c>
       <c r="F31">
         <f>44.45+F30</f>
-        <v>49.729059037199249</v>
+        <v>49.675934037199248</v>
       </c>
       <c r="G31">
         <f>50.71+G30</f>
-        <v>50.306039171559107</v>
+        <v>50.252914171559112</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Forecasts for Independents now incorporates seat betting odds.
</commit_message>
<xml_diff>
--- a/Temporary Region Swings.xlsx
+++ b/Temporary Region Swings.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54418CA0-BBB6-423A-AD9C-57A0F473CC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F584D3C-8A86-47C1-80EE-4DAE70732986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="4965" windowWidth="24255" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9945" yWindow="5235" windowWidth="24255" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="1" r:id="rId1"/>
     <sheet name="Archives" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -480,7 +481,7 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,22 +640,22 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>56.5</v>
+        <v>56</v>
       </c>
       <c r="C6">
-        <v>55.5</v>
+        <v>58</v>
       </c>
       <c r="D6">
-        <v>58.5</v>
+        <v>59</v>
       </c>
       <c r="E6">
-        <v>54.5</v>
+        <v>48.5</v>
       </c>
       <c r="F6">
         <v>50.5</v>
       </c>
       <c r="G6">
-        <v>64.5</v>
+        <v>60.5</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -665,19 +666,19 @@
         <v>55.5</v>
       </c>
       <c r="C7">
-        <v>55.5</v>
+        <v>56.5</v>
       </c>
       <c r="D7">
-        <v>58</v>
+        <v>57.5</v>
       </c>
       <c r="E7">
-        <v>51.5</v>
+        <v>50.5</v>
       </c>
       <c r="F7">
-        <v>53.5</v>
+        <v>53</v>
       </c>
       <c r="G7">
-        <v>55.5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -685,22 +686,22 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>53.5</v>
+        <v>56.5</v>
       </c>
       <c r="C8">
-        <v>53.5</v>
+        <v>55.5</v>
       </c>
       <c r="D8">
-        <v>55</v>
+        <v>58.5</v>
       </c>
       <c r="E8">
-        <v>47</v>
+        <v>54.5</v>
       </c>
       <c r="F8">
-        <v>53.5</v>
+        <v>50.5</v>
       </c>
       <c r="G8">
-        <v>57.5</v>
+        <v>64.5</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -935,27 +936,27 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>-0.75</v>
+        <v>2.25</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>-2.6700000000000017</v>
+        <v>-1.6700000000000017</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>4.9099999999999966</v>
+        <v>-0.59000000000000341</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>-1.980000000000004</v>
+        <v>-1.480000000000004</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>5.759999999999998</v>
+        <v>2.259999999999998</v>
       </c>
       <c r="H19" s="2">
         <f>F19*0.439183+G19*0.336042</f>
-        <v>1.0660195799999976</v>
+        <v>0.10946407999999763</v>
       </c>
       <c r="J19">
         <v>1401874</v>
@@ -979,27 +980,27 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>-2.1700000000000017</v>
+        <v>-2.6700000000000017</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>2.9099999999999966</v>
+        <v>1.9099999999999966</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>2.019999999999996</v>
+        <v>1.519999999999996</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
-        <v>-2.240000000000002</v>
+        <v>2.259999999999998</v>
       </c>
       <c r="H20" s="2">
         <f>F20*0.439183+G20*0.336042</f>
-        <v>0.13441557999999765</v>
+        <v>1.4270130799999976</v>
       </c>
       <c r="J20">
         <f>J19/SUM($J19:$N19)</f>
@@ -1016,27 +1017,27 @@
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>-3.1700000000000017</v>
+        <v>-2.6700000000000017</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>0.40999999999999659</v>
+        <v>4.9099999999999966</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>4.019999999999996</v>
+        <v>-1.980000000000004</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
-        <v>1.759999999999998</v>
+        <v>5.759999999999998</v>
       </c>
       <c r="H21" s="2">
         <f>F21*0.439183+G21*0.336042</f>
-        <v>2.3569495799999975</v>
+        <v>1.0660195799999976</v>
       </c>
       <c r="L21">
         <f>(J19+K19)/SUM(J19:N19)</f>
@@ -1061,11 +1062,11 @@
       </c>
       <c r="F22" s="2">
         <f t="shared" ref="F22:G24" si="2">AVERAGE(F$18,F$18,F$18,F$18,F$18,F$18,F$19,F$20,F$21)+($H22-AVERAGE($H$18,$H$18,$H$18,$H$18,$H$18,$H$18,$H$19,$H$20,$H$21))</f>
-        <v>1.6268596203419832</v>
+        <v>1.0662916203419837</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="2"/>
-        <v>-2.410918157435793</v>
+        <v>-1.7492639352135697</v>
       </c>
       <c r="H22">
         <f>(H9-H$2)-($B9-$B$2)</f>
@@ -1090,11 +1091,11 @@
       </c>
       <c r="F23" s="2">
         <f t="shared" si="2"/>
-        <v>5.7798596203419894</v>
+        <v>5.2192916203419895</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="2"/>
-        <v>1.7420818425642131</v>
+        <v>2.4037360647864356</v>
       </c>
       <c r="H23">
         <f>(H10-H$2)-($B10-$B$2)</f>
@@ -1119,11 +1120,11 @@
       </c>
       <c r="F24" s="2">
         <f t="shared" si="2"/>
-        <v>4.1388596203419841</v>
+        <v>3.5782916203419841</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" si="2"/>
-        <v>0.10108184256420766</v>
+        <v>0.76273606478643041</v>
       </c>
       <c r="H24">
         <f>(H11-H$2)-($B11-$B$2)</f>
@@ -1249,45 +1250,45 @@
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C30">
         <f>AVERAGE(C18,C18,C18,C18,C18,C18,C19,C20,C21,C22,C23,C24,C25,C26,C27,C28)</f>
-        <v>-0.9263896100119875</v>
+        <v>-0.7388896100119875</v>
       </c>
       <c r="D30">
         <f>AVERAGE(D18,D18,D18,D18,D18,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28)</f>
-        <v>-2.4018656930940945</v>
+        <v>-2.3393656930940945</v>
       </c>
       <c r="E30">
         <f>AVERAGE(E18,E18,E18,E18,E18,E18,E19,E20,E21,E22,E23,E24,E25,E26,E27,E28)</f>
-        <v>3.7202088500435218</v>
+        <v>3.5952088500435218</v>
       </c>
       <c r="F30">
         <f>AVERAGE(F18,F18,F18,F18,F18,F18,F19,F20,F21,F22,F23,F24,F25,F26,F27,F28)</f>
-        <v>5.225934037199246</v>
+        <v>4.7458275371992471</v>
       </c>
       <c r="G30">
         <f>AVERAGE(G18,G18,G18,G18,G18,G18,G19,G20,G21,G22,G23,G24,G25,G26,G27,G28)</f>
-        <v>-0.45708582844089174</v>
+        <v>-2.0525661774224879E-2</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C31">
         <f>48.22+C30</f>
-        <v>47.293610389988011</v>
+        <v>47.481110389988011</v>
       </c>
       <c r="D31">
         <f>53.14+D30</f>
-        <v>50.738134306905906</v>
+        <v>50.800634306905906</v>
       </c>
       <c r="E31">
         <f>41.56+E30</f>
-        <v>45.280208850043522</v>
+        <v>45.155208850043522</v>
       </c>
       <c r="F31">
         <f>44.45+F30</f>
-        <v>49.675934037199248</v>
+        <v>49.19582753719925</v>
       </c>
       <c r="G31">
         <f>50.71+G30</f>
-        <v>50.252914171559112</v>
+        <v>50.689474338225779</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update for Essential poll
</commit_message>
<xml_diff>
--- a/Temporary Region Swings.xlsx
+++ b/Temporary Region Swings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DA84C0-7860-40BE-85CE-FD3AA5C7AD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E213C90-37C7-4348-8230-09FFC140F2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5625" yWindow="5550" windowWidth="24255" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="5955" windowWidth="24255" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
   <si>
     <t>NSW</t>
   </si>
@@ -136,10 +136,10 @@
     <t>Second Essential -&gt;</t>
   </si>
   <si>
-    <t>Third Essential -&gt;</t>
-  </si>
-  <si>
-    <t>Fourth Essential -&gt;</t>
+    <t>Latest Essential (3 avg.) -&gt;</t>
+  </si>
+  <si>
+    <t>Second Essential (3 avg.) -&gt;</t>
   </si>
 </sst>
 </file>
@@ -477,15 +477,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -657,22 +657,22 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>56</v>
+        <v>56.5</v>
       </c>
       <c r="C6">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D6">
         <v>59</v>
       </c>
       <c r="E6">
-        <v>48.5</v>
+        <v>51.5</v>
       </c>
       <c r="F6">
-        <v>50.5</v>
+        <v>55.5</v>
       </c>
       <c r="G6">
-        <v>60.5</v>
+        <v>64</v>
       </c>
       <c r="J6">
         <v>29.951599999999999</v>
@@ -702,22 +702,22 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>55.5</v>
+        <v>56</v>
       </c>
       <c r="C7">
-        <v>56.5</v>
+        <v>58</v>
       </c>
       <c r="D7">
-        <v>57.5</v>
+        <v>59</v>
       </c>
       <c r="E7">
+        <v>48.5</v>
+      </c>
+      <c r="F7">
         <v>50.5</v>
       </c>
-      <c r="F7">
-        <v>53</v>
-      </c>
       <c r="G7">
-        <v>60</v>
+        <v>60.5</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -725,22 +725,22 @@
         <v>10</v>
       </c>
       <c r="B8">
+        <v>55.5</v>
+      </c>
+      <c r="C8">
         <v>56.5</v>
       </c>
-      <c r="C8">
-        <v>55.5</v>
-      </c>
       <c r="D8">
-        <v>58.5</v>
+        <v>57.5</v>
       </c>
       <c r="E8">
-        <v>54.5</v>
+        <v>50.5</v>
       </c>
       <c r="F8">
-        <v>50.5</v>
+        <v>53</v>
       </c>
       <c r="G8">
-        <v>64.5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -805,544 +805,440 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B12">
-        <v>51.612903225806448</v>
+        <v>52.158273381294961</v>
       </c>
       <c r="C12">
-        <v>45.161290322580648</v>
+        <v>49.81818181818182</v>
       </c>
       <c r="D12">
-        <v>48.421052631578945</v>
+        <v>53.763440860215056</v>
       </c>
       <c r="E12">
-        <v>60.638297872340424</v>
+        <v>50.183150183150182</v>
       </c>
       <c r="F12">
-        <v>54.838709677419352</v>
+        <v>57.446808510638299</v>
       </c>
       <c r="G12">
-        <v>48.936170212765958</v>
+        <v>48.913043478260867</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B13">
-        <v>51.111111111111114</v>
+        <v>51.272727272727273</v>
       </c>
       <c r="C13">
-        <v>50</v>
+        <v>47.636363636363633</v>
       </c>
       <c r="D13">
-        <v>50</v>
+        <v>49.819494584837543</v>
       </c>
       <c r="E13">
-        <v>55.172413793103445</v>
+        <v>55.839416058394164</v>
       </c>
       <c r="F13">
-        <v>52.688172043010752</v>
+        <v>53.763440860215056</v>
       </c>
       <c r="G13">
-        <v>50.549450549450547</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14">
-        <v>52.688172039999998</v>
-      </c>
-      <c r="C14">
         <v>49.462365591397848</v>
       </c>
-      <c r="D14">
-        <v>55.319148936170215</v>
-      </c>
-      <c r="E14">
-        <v>51.612903225806448</v>
-      </c>
-      <c r="F14">
-        <v>53.191489361702125</v>
-      </c>
-      <c r="G14">
-        <v>53.763440860215056</v>
-      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15">
-        <v>50.549450550000003</v>
-      </c>
-      <c r="C15">
-        <v>47.252747252747255</v>
-      </c>
-      <c r="D15">
-        <v>53.932584269662918</v>
-      </c>
-      <c r="E15">
-        <v>51.136363636363633</v>
-      </c>
-      <c r="F15">
-        <v>61.05263157894737</v>
-      </c>
-      <c r="G15">
-        <v>51.086956521739133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C15" t="s">
         <v>0</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D15" t="s">
         <v>1</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E15" t="s">
         <v>2</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F15" t="s">
         <v>4</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G15" t="s">
         <v>3</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <f>(C5-C$2)-($B5-$B$2)</f>
+        <v>0.25</v>
+      </c>
+      <c r="D16">
+        <f>(D5-D$2)-($B5-$B$2)</f>
+        <v>-1.6700000000000017</v>
+      </c>
+      <c r="E16">
+        <f>(E5-E$2)-($B5-$B$2)</f>
+        <v>-9.0000000000003411E-2</v>
+      </c>
+      <c r="F16">
+        <f>(F5-F$2)-($B5-$B$2)</f>
+        <v>6.019999999999996</v>
+      </c>
+      <c r="G16">
+        <f>(G5-G$2)-($B5-$B$2)</f>
+        <v>-0.24000000000000199</v>
+      </c>
+      <c r="H16" s="2">
+        <f>F16*0.439183+G16*0.336042</f>
+        <v>2.5632315799999974</v>
+      </c>
+      <c r="J16">
+        <v>44.45</v>
+      </c>
+      <c r="K16">
+        <v>50.71</v>
+      </c>
+      <c r="L16">
+        <v>55.96</v>
+      </c>
+      <c r="M16">
+        <v>61.61</v>
+      </c>
+      <c r="N16">
+        <v>54.2</v>
+      </c>
+      <c r="P16">
+        <f>(J16*J17+K16*K17+L16*L17+M16*M17+N16*N17)/SUM(J17:N17)</f>
+        <v>49.554498799658013</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <f>(C6-C$2)-($B6-$B$2)</f>
+        <v>-2.25</v>
+      </c>
+      <c r="D17">
+        <f>(D6-D$2)-($B6-$B$2)</f>
+        <v>-2.1700000000000017</v>
+      </c>
+      <c r="E17">
+        <f>(E6-E$2)-($B6-$B$2)</f>
+        <v>1.9099999999999966</v>
+      </c>
+      <c r="F17">
+        <f>(F6-F$2)-($B6-$B$2)</f>
+        <v>3.019999999999996</v>
+      </c>
+      <c r="G17">
+        <f>(G6-G$2)-($B6-$B$2)</f>
+        <v>5.259999999999998</v>
+      </c>
+      <c r="H17" s="2">
+        <f>F17*0.439183+G17*0.336042</f>
+        <v>3.0939135799999979</v>
+      </c>
+      <c r="J17">
+        <v>1401874</v>
+      </c>
+      <c r="K17">
+        <v>1072648</v>
+      </c>
+      <c r="L17">
+        <v>347992</v>
+      </c>
+      <c r="M17">
+        <v>265975</v>
+      </c>
+      <c r="N17">
+        <v>103518</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:G21" si="0">(C5-C$2)-($B5-$B$2)</f>
-        <v>0.25</v>
+        <f>(C7-C$2)-($B7-$B$2)</f>
+        <v>2.25</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f>(D7-D$2)-($B7-$B$2)</f>
         <v>-1.6700000000000017</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
-        <v>-9.0000000000003411E-2</v>
+        <f>(E7-E$2)-($B7-$B$2)</f>
+        <v>-0.59000000000000341</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
-        <v>6.019999999999996</v>
+        <f>(F7-F$2)-($B7-$B$2)</f>
+        <v>-1.480000000000004</v>
       </c>
       <c r="G18">
-        <f t="shared" si="0"/>
-        <v>-0.24000000000000199</v>
+        <f>(G7-G$2)-($B7-$B$2)</f>
+        <v>2.259999999999998</v>
       </c>
       <c r="H18" s="2">
         <f>F18*0.439183+G18*0.336042</f>
-        <v>2.5632315799999974</v>
+        <v>0.10946407999999763</v>
       </c>
       <c r="J18">
-        <v>44.45</v>
+        <f>J17/SUM($J17:$N17)</f>
+        <v>0.43918262084011722</v>
       </c>
       <c r="K18">
-        <v>50.71</v>
-      </c>
-      <c r="L18">
-        <v>55.96</v>
-      </c>
-      <c r="M18">
-        <v>61.61</v>
-      </c>
-      <c r="N18">
-        <v>54.2</v>
-      </c>
-      <c r="P18">
-        <f>(J18*J19+K18*K19+L18*L19+M18*M19+N18*N19)/SUM(J19:N19)</f>
-        <v>49.554498799658013</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <f>K17/SUM($J17:$N17)</f>
+        <v>0.3360418695823662</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
-        <v>2.25</v>
+        <f>(C8-C$2)-($B8-$B$2)</f>
+        <v>1.25</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
-        <v>-1.6700000000000017</v>
+        <f>(D8-D$2)-($B8-$B$2)</f>
+        <v>-2.6700000000000017</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
-        <v>-0.59000000000000341</v>
+        <f>(E8-E$2)-($B8-$B$2)</f>
+        <v>1.9099999999999966</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
-        <v>-1.480000000000004</v>
+        <f>(F8-F$2)-($B8-$B$2)</f>
+        <v>1.519999999999996</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
+        <f>(G8-G$2)-($B8-$B$2)</f>
         <v>2.259999999999998</v>
       </c>
       <c r="H19" s="2">
         <f>F19*0.439183+G19*0.336042</f>
-        <v>0.10946407999999763</v>
-      </c>
-      <c r="J19">
-        <v>1401874</v>
-      </c>
-      <c r="K19">
-        <v>1072648</v>
+        <v>1.4270130799999976</v>
       </c>
       <c r="L19">
-        <v>347992</v>
-      </c>
-      <c r="M19">
-        <v>265975</v>
-      </c>
-      <c r="N19">
-        <v>103518</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+        <f>(J17+K17)/SUM(J17:N17)</f>
+        <v>0.77522449042248343</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C20">
+        <f>(C9-C$2)-($B9-$B$2)</f>
+        <v>-1.1229999999999976</v>
+      </c>
+      <c r="D20">
+        <f>(D9-D$2)-($B9-$B$2)</f>
+        <v>0.14099999999999824</v>
+      </c>
+      <c r="E20">
+        <f>(E9-E$2)-($B9-$B$2)</f>
+        <v>2.1430000000000007</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" ref="F20:G22" si="0">AVERAGE(F$16,F$16,F$16,F$16,F$16,F$16,F$17,F$18,F$19)+($H20-AVERAGE($H$16,$H$16,$H$16,$H$16,$H$16,$H$16,$H$17,$H$18,$H$19))</f>
+        <v>1.3965256203419827</v>
+      </c>
+      <c r="G20" s="2">
         <f t="shared" si="0"/>
-        <v>1.25</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>-2.6700000000000017</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>1.9099999999999966</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>1.519999999999996</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="0"/>
-        <v>2.259999999999998</v>
-      </c>
-      <c r="H20" s="2">
-        <f>F20*0.439183+G20*0.336042</f>
-        <v>1.4270130799999976</v>
-      </c>
-      <c r="J20">
-        <f>J19/SUM($J19:$N19)</f>
-        <v>0.43918262084011722</v>
-      </c>
-      <c r="K20">
-        <f>K19/SUM($J19:$N19)</f>
-        <v>0.3360418695823662</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="0"/>
-        <v>-0.75</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>-2.6700000000000017</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>4.9099999999999966</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>-1.980000000000004</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="0"/>
-        <v>5.759999999999998</v>
-      </c>
-      <c r="H21" s="2">
-        <f>F21*0.439183+G21*0.336042</f>
-        <v>1.0660195799999976</v>
-      </c>
-      <c r="L21">
-        <f>(J19+K19)/SUM(J19:N19)</f>
-        <v>0.77522449042248343</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22">
-        <f t="shared" ref="C22:E26" si="1">(C9-C$2)-($B9-$B$2)</f>
-        <v>-1.1229999999999976</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="1"/>
-        <v>0.14099999999999824</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="1"/>
-        <v>2.1430000000000007</v>
-      </c>
-      <c r="F22" s="2">
-        <f t="shared" ref="F22:G24" si="2">AVERAGE(F$18,F$18,F$18,F$18,F$18,F$18,F$19,F$20,F$21)+($H22-AVERAGE($H$18,$H$18,$H$18,$H$18,$H$18,$H$18,$H$19,$H$20,$H$21))</f>
-        <v>1.0662916203419837</v>
-      </c>
-      <c r="G22" s="2">
-        <f t="shared" si="2"/>
-        <v>-1.7492639352135697</v>
-      </c>
-      <c r="H22">
+        <v>-2.0301410463246818</v>
+      </c>
+      <c r="H20">
         <f>(H9-H$2)-($B9-$B$2)</f>
         <v>-0.73349879965801534</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="C23">
-        <f t="shared" si="1"/>
+      <c r="C21">
+        <f>(C10-C$2)-($B10-$B$2)</f>
         <v>-1.5769999999999982</v>
       </c>
-      <c r="D23">
-        <f t="shared" si="1"/>
+      <c r="D21">
+        <f>(D10-D$2)-($B10-$B$2)</f>
         <v>-0.37100000000000222</v>
       </c>
-      <c r="E23">
-        <f t="shared" si="1"/>
+      <c r="E21">
+        <f>(E10-E$2)-($B10-$B$2)</f>
         <v>3.2929999999999993</v>
       </c>
-      <c r="F23" s="2">
-        <f t="shared" si="2"/>
-        <v>5.2192916203419895</v>
-      </c>
-      <c r="G23" s="2">
-        <f t="shared" si="2"/>
-        <v>2.4037360647864356</v>
-      </c>
-      <c r="H23">
+      <c r="F21" s="2">
+        <f t="shared" si="0"/>
+        <v>5.5495256203419885</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>2.122858953675324</v>
+      </c>
+      <c r="H21">
         <f>(H10-H$2)-($B10-$B$2)</f>
         <v>3.4195012003419905</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="C24">
-        <f t="shared" si="1"/>
+      <c r="C22">
+        <f>(C11-C$2)-($B11-$B$2)</f>
         <v>-0.28699999999999193</v>
       </c>
-      <c r="D24">
-        <f t="shared" si="1"/>
+      <c r="D22">
+        <f>(D11-D$2)-($B11-$B$2)</f>
         <v>-3.2010000000000005</v>
       </c>
-      <c r="E24">
-        <f t="shared" si="1"/>
+      <c r="E22">
+        <f>(E11-E$2)-($B11-$B$2)</f>
         <v>6.159000000000006</v>
       </c>
-      <c r="F24" s="2">
-        <f t="shared" si="2"/>
-        <v>3.5782916203419841</v>
-      </c>
-      <c r="G24" s="2">
-        <f t="shared" si="2"/>
-        <v>0.76273606478643041</v>
-      </c>
-      <c r="H24">
+      <c r="F22" s="2">
+        <f t="shared" si="0"/>
+        <v>3.9085256203419831</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.48185895367531872</v>
+      </c>
+      <c r="H22">
         <f>(H11-H$2)-($B11-$B$2)</f>
         <v>1.7785012003419851</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>31</v>
       </c>
-      <c r="C25">
-        <f t="shared" si="1"/>
-        <v>-6.2016129032258007</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="1"/>
-        <v>-7.861850594227505</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="1"/>
-        <v>15.935394646533972</v>
-      </c>
-      <c r="F25">
+      <c r="C23">
+        <f>(C12-C$2)-($B12-$B$2)</f>
+        <v>-2.0900915631131411</v>
+      </c>
+      <c r="D23">
+        <f>(D12-D$2)-($B12-$B$2)</f>
+        <v>-3.0648325210799072</v>
+      </c>
+      <c r="E23">
+        <f>(E12-E$2)-($B12-$B$2)</f>
+        <v>4.9348768018552178</v>
+      </c>
+      <c r="F23">
         <f>(F12-F$2)-($B12-$B$2)</f>
-        <v>7.2458064516128999</v>
-      </c>
-      <c r="G25">
+        <v>9.3085351293433334</v>
+      </c>
+      <c r="G23">
         <f>(G12-G$2)-($B12-$B$2)</f>
-        <v>-4.916733013040492</v>
-      </c>
-      <c r="H25" s="2">
-        <f>F25*0.439183+G25*0.336042</f>
-        <v>1.5300062196705548</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+        <v>-5.4852299030340959</v>
+      </c>
+      <c r="H23" s="2">
+        <f>F23*0.439183+G23*0.336042</f>
+        <v>2.2448827566350094</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>32</v>
       </c>
+      <c r="C24">
+        <f>(C13-C$2)-($B13-$B$2)</f>
+        <v>-3.3863636363636402</v>
+      </c>
+      <c r="D24">
+        <f>(D13-D$2)-($B13-$B$2)</f>
+        <v>-6.1232326878897325</v>
+      </c>
+      <c r="E24">
+        <f>(E13-E$2)-($B13-$B$2)</f>
+        <v>11.476688785666887</v>
+      </c>
+      <c r="F24">
+        <f>(F13-F$2)-($B13-$B$2)</f>
+        <v>6.5107135874877784</v>
+      </c>
+      <c r="G24">
+        <f>(G13-G$2)-($B13-$B$2)</f>
+        <v>-4.0503616813294272</v>
+      </c>
+      <c r="H24" s="2">
+        <f>F24*0.439183+G24*0.336042</f>
+        <v>1.4983030853763413</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C26">
-        <f t="shared" si="1"/>
-        <v>-0.86111111111111427</v>
+        <f>AVERAGE(C16,C16,AVERAGE(C17,C18,C19),AVERAGE(C20,C21,C22),AVERAGE(C23,C24))</f>
+        <v>-0.56344551994767733</v>
       </c>
       <c r="D26">
-        <f t="shared" si="1"/>
-        <v>-5.781111111111116</v>
+        <f t="shared" ref="D26:G26" si="1">AVERAGE(D16,D16,AVERAGE(D17,D18,D19),AVERAGE(D20,D21,D22),AVERAGE(D23,D24))</f>
+        <v>-2.2495398542302985</v>
       </c>
       <c r="E26">
         <f t="shared" si="1"/>
-        <v>10.971302681992327</v>
+        <v>2.5934898920855423</v>
       </c>
       <c r="F26">
-        <f>(F13-F$2)-($B13-$B$2)</f>
-        <v>5.5970609318996338</v>
+        <f t="shared" si="1"/>
+        <v>4.9175633290848388</v>
       </c>
       <c r="G26">
-        <f>(G13-G$2)-($B13-$B$2)</f>
-        <v>-2.8016605616605688</v>
-      </c>
-      <c r="H26" s="2">
-        <f>F26*0.439183+G26*0.336042</f>
-        <v>1.516658392792936</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>33</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>-0.35925403436795611</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C27">
-        <f t="shared" ref="C27:G28" si="3">(C14-C$2)-($B14-$B$2)</f>
-        <v>-2.9758064486021496</v>
+        <f>48.22+C26</f>
+        <v>47.656554480052321</v>
       </c>
       <c r="D27">
-        <f t="shared" si="3"/>
-        <v>-2.0390231038297841</v>
+        <f>53.14+D26</f>
+        <v>50.890460145769701</v>
       </c>
       <c r="E27">
-        <f t="shared" si="3"/>
-        <v>5.8347311858064472</v>
+        <f>41.56+E26</f>
+        <v>44.153489892085545</v>
       </c>
       <c r="F27">
-        <f t="shared" si="3"/>
-        <v>4.5233173217021232</v>
+        <f>44.45+F26</f>
+        <v>49.367563329084845</v>
       </c>
       <c r="G27">
-        <f t="shared" si="3"/>
-        <v>-1.164731179784944</v>
-      </c>
-      <c r="H27" s="2">
-        <f>F27*0.439183+G27*0.336042</f>
-        <v>1.5951654761798113</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="3"/>
-        <v>-3.0467032972527477</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="3"/>
-        <v>-1.2868662803370867</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="3"/>
-        <v>7.4969130863636266</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="3"/>
-        <v>14.523181028947363</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="3"/>
-        <v>-1.7024940282608725</v>
-      </c>
-      <c r="H28" s="2">
-        <f>F28*0.439183+G28*0.336042</f>
-        <v>5.8062247155913491</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C30">
-        <f>AVERAGE(C18,C18,C18,C18,C18,C18,C19,C20,C21,C22,C23,C24,C25,C26,C27,C28)</f>
-        <v>-0.7388896100119875</v>
-      </c>
-      <c r="D30">
-        <f>AVERAGE(D18,D18,D18,D18,D18,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28)</f>
-        <v>-2.3393656930940945</v>
-      </c>
-      <c r="E30">
-        <f>AVERAGE(E18,E18,E18,E18,E18,E18,E19,E20,E21,E22,E23,E24,E25,E26,E27,E28)</f>
-        <v>3.5952088500435218</v>
-      </c>
-      <c r="F30">
-        <f>AVERAGE(F18,F18,F18,F18,F18,F18,F19,F20,F21,F22,F23,F24,F25,F26,F27,F28)</f>
-        <v>4.7458275371992471</v>
-      </c>
-      <c r="G30">
-        <f>AVERAGE(G18,G18,G18,G18,G18,G18,G19,G20,G21,G22,G23,G24,G25,G26,G27,G28)</f>
-        <v>-2.0525661774224879E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C31">
-        <f>48.22+C30</f>
-        <v>47.481110389988011</v>
-      </c>
-      <c r="D31">
-        <f>53.14+D30</f>
-        <v>50.800634306905906</v>
-      </c>
-      <c r="E31">
-        <f>41.56+E30</f>
-        <v>45.155208850043522</v>
-      </c>
-      <c r="F31">
-        <f>44.45+F30</f>
-        <v>49.19582753719925</v>
-      </c>
-      <c r="G31">
-        <f>50.71+G30</f>
-        <v>50.689474338225779</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38">
+        <f>50.71+G26</f>
+        <v>50.350745965632044</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
         <f>9.26*0.832</f>
         <v>7.7043199999999992</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
         <f>20.48*0.619</f>
         <v>12.67712</v>
       </c>
-      <c r="B39">
-        <f>(A39-A38)/(20.48-9.26)</f>
+      <c r="B35">
+        <f>(A35-A34)/(20.48-9.26)</f>
         <v>0.4432085561497327</v>
       </c>
     </row>
@@ -1360,7 +1256,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update for numerous new polls.
</commit_message>
<xml_diff>
--- a/Temporary Region Swings.xlsx
+++ b/Temporary Region Swings.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E213C90-37C7-4348-8230-09FFC140F2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BFCCD8-9762-456A-B9CF-E290850FAA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="5955" windowWidth="24255" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="4455" windowWidth="24255" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="1" r:id="rId1"/>
     <sheet name="Archives" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -480,7 +481,7 @@
   <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,22 +658,22 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>56.5</v>
+        <v>57</v>
       </c>
       <c r="C6">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D6">
-        <v>59</v>
+        <v>57.5</v>
       </c>
       <c r="E6">
         <v>51.5</v>
       </c>
       <c r="F6">
-        <v>55.5</v>
+        <v>53.5</v>
       </c>
       <c r="G6">
-        <v>64</v>
+        <v>59.5</v>
       </c>
       <c r="J6">
         <v>29.951599999999999</v>
@@ -702,22 +703,22 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>56</v>
+        <v>56.5</v>
       </c>
       <c r="C7">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D7">
         <v>59</v>
       </c>
       <c r="E7">
-        <v>48.5</v>
+        <v>51.5</v>
       </c>
       <c r="F7">
-        <v>50.5</v>
+        <v>55.5</v>
       </c>
       <c r="G7">
-        <v>60.5</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -725,22 +726,22 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>55.5</v>
+        <v>56</v>
       </c>
       <c r="C8">
-        <v>56.5</v>
+        <v>58</v>
       </c>
       <c r="D8">
-        <v>57.5</v>
+        <v>59</v>
       </c>
       <c r="E8">
+        <v>48.5</v>
+      </c>
+      <c r="F8">
         <v>50.5</v>
       </c>
-      <c r="F8">
-        <v>53</v>
-      </c>
       <c r="G8">
-        <v>60</v>
+        <v>60.5</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -808,22 +809,22 @@
         <v>33</v>
       </c>
       <c r="B12">
-        <v>52.158273381294961</v>
+        <v>52.142857142857139</v>
       </c>
       <c r="C12">
-        <v>49.81818181818182</v>
+        <v>49.635036496350367</v>
       </c>
       <c r="D12">
-        <v>53.763440860215056</v>
+        <v>52.857142857142861</v>
       </c>
       <c r="E12">
-        <v>50.183150183150182</v>
+        <v>51.957295373665481</v>
       </c>
       <c r="F12">
-        <v>57.446808510638299</v>
+        <v>54.255319148936174</v>
       </c>
       <c r="G12">
-        <v>48.913043478260867</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -831,22 +832,22 @@
         <v>34</v>
       </c>
       <c r="B13">
-        <v>51.272727272727273</v>
+        <v>51.624548736462089</v>
       </c>
       <c r="C13">
-        <v>47.636363636363633</v>
+        <v>47.653429602888082</v>
       </c>
       <c r="D13">
-        <v>49.819494584837543</v>
+        <v>50.719424460431661</v>
       </c>
       <c r="E13">
-        <v>55.839416058394164</v>
+        <v>53.429602888086642</v>
       </c>
       <c r="F13">
-        <v>53.763440860215056</v>
+        <v>59.574468085106382</v>
       </c>
       <c r="G13">
-        <v>49.462365591397848</v>
+        <v>50.537634408602152</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -880,23 +881,23 @@
         <v>7</v>
       </c>
       <c r="C16">
-        <f>(C5-C$2)-($B5-$B$2)</f>
+        <f t="shared" ref="C16:G19" si="0">(C5-C$2)-($B5-$B$2)</f>
         <v>0.25</v>
       </c>
       <c r="D16">
-        <f>(D5-D$2)-($B5-$B$2)</f>
+        <f t="shared" si="0"/>
         <v>-1.6700000000000017</v>
       </c>
       <c r="E16">
-        <f>(E5-E$2)-($B5-$B$2)</f>
+        <f t="shared" si="0"/>
         <v>-9.0000000000003411E-2</v>
       </c>
       <c r="F16">
-        <f>(F5-F$2)-($B5-$B$2)</f>
+        <f t="shared" si="0"/>
         <v>6.019999999999996</v>
       </c>
       <c r="G16">
-        <f>(G5-G$2)-($B5-$B$2)</f>
+        <f t="shared" si="0"/>
         <v>-0.24000000000000199</v>
       </c>
       <c r="H16" s="2">
@@ -928,28 +929,28 @@
         <v>8</v>
       </c>
       <c r="C17">
-        <f>(C6-C$2)-($B6-$B$2)</f>
-        <v>-2.25</v>
+        <f t="shared" si="0"/>
+        <v>2.25</v>
       </c>
       <c r="D17">
-        <f>(D6-D$2)-($B6-$B$2)</f>
-        <v>-2.1700000000000017</v>
+        <f t="shared" si="0"/>
+        <v>-4.1700000000000017</v>
       </c>
       <c r="E17">
-        <f>(E6-E$2)-($B6-$B$2)</f>
-        <v>1.9099999999999966</v>
+        <f t="shared" si="0"/>
+        <v>1.4099999999999966</v>
       </c>
       <c r="F17">
-        <f>(F6-F$2)-($B6-$B$2)</f>
-        <v>3.019999999999996</v>
+        <f t="shared" si="0"/>
+        <v>0.51999999999999602</v>
       </c>
       <c r="G17">
-        <f>(G6-G$2)-($B6-$B$2)</f>
-        <v>5.259999999999998</v>
+        <f t="shared" si="0"/>
+        <v>0.25999999999999801</v>
       </c>
       <c r="H17" s="2">
         <f>F17*0.439183+G17*0.336042</f>
-        <v>3.0939135799999979</v>
+        <v>0.3157460799999976</v>
       </c>
       <c r="J17">
         <v>1401874</v>
@@ -972,28 +973,28 @@
         <v>9</v>
       </c>
       <c r="C18">
-        <f>(C7-C$2)-($B7-$B$2)</f>
-        <v>2.25</v>
+        <f t="shared" si="0"/>
+        <v>-2.25</v>
       </c>
       <c r="D18">
-        <f>(D7-D$2)-($B7-$B$2)</f>
-        <v>-1.6700000000000017</v>
+        <f t="shared" si="0"/>
+        <v>-2.1700000000000017</v>
       </c>
       <c r="E18">
-        <f>(E7-E$2)-($B7-$B$2)</f>
-        <v>-0.59000000000000341</v>
+        <f t="shared" si="0"/>
+        <v>1.9099999999999966</v>
       </c>
       <c r="F18">
-        <f>(F7-F$2)-($B7-$B$2)</f>
-        <v>-1.480000000000004</v>
+        <f t="shared" si="0"/>
+        <v>3.019999999999996</v>
       </c>
       <c r="G18">
-        <f>(G7-G$2)-($B7-$B$2)</f>
-        <v>2.259999999999998</v>
+        <f t="shared" si="0"/>
+        <v>5.259999999999998</v>
       </c>
       <c r="H18" s="2">
         <f>F18*0.439183+G18*0.336042</f>
-        <v>0.10946407999999763</v>
+        <v>3.0939135799999979</v>
       </c>
       <c r="J18">
         <f>J17/SUM($J17:$N17)</f>
@@ -1009,28 +1010,28 @@
         <v>10</v>
       </c>
       <c r="C19">
-        <f>(C8-C$2)-($B8-$B$2)</f>
-        <v>1.25</v>
+        <f t="shared" si="0"/>
+        <v>2.25</v>
       </c>
       <c r="D19">
-        <f>(D8-D$2)-($B8-$B$2)</f>
-        <v>-2.6700000000000017</v>
+        <f t="shared" si="0"/>
+        <v>-1.6700000000000017</v>
       </c>
       <c r="E19">
-        <f>(E8-E$2)-($B8-$B$2)</f>
-        <v>1.9099999999999966</v>
+        <f t="shared" si="0"/>
+        <v>-0.59000000000000341</v>
       </c>
       <c r="F19">
-        <f>(F8-F$2)-($B8-$B$2)</f>
-        <v>1.519999999999996</v>
+        <f t="shared" si="0"/>
+        <v>-1.480000000000004</v>
       </c>
       <c r="G19">
-        <f>(G8-G$2)-($B8-$B$2)</f>
+        <f t="shared" si="0"/>
         <v>2.259999999999998</v>
       </c>
       <c r="H19" s="2">
         <f>F19*0.439183+G19*0.336042</f>
-        <v>1.4270130799999976</v>
+        <v>0.10946407999999763</v>
       </c>
       <c r="L19">
         <f>(J17+K17)/SUM(J17:N17)</f>
@@ -1042,24 +1043,24 @@
         <v>11</v>
       </c>
       <c r="C20">
-        <f>(C9-C$2)-($B9-$B$2)</f>
+        <f t="shared" ref="C20:E24" si="1">(C9-C$2)-($B9-$B$2)</f>
         <v>-1.1229999999999976</v>
       </c>
       <c r="D20">
-        <f>(D9-D$2)-($B9-$B$2)</f>
+        <f t="shared" si="1"/>
         <v>0.14099999999999824</v>
       </c>
       <c r="E20">
-        <f>(E9-E$2)-($B9-$B$2)</f>
+        <f t="shared" si="1"/>
         <v>2.1430000000000007</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" ref="F20:G22" si="0">AVERAGE(F$16,F$16,F$16,F$16,F$16,F$16,F$17,F$18,F$19)+($H20-AVERAGE($H$16,$H$16,$H$16,$H$16,$H$16,$H$16,$H$17,$H$18,$H$19))</f>
-        <v>1.3965256203419827</v>
+        <f t="shared" ref="F20:G22" si="2">AVERAGE(F$16,F$16,F$16,F$16,F$16,F$16,F$17,F$18,F$19)+($H20-AVERAGE($H$16,$H$16,$H$16,$H$16,$H$16,$H$16,$H$17,$H$18,$H$19))</f>
+        <v>1.4088886203419833</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="0"/>
-        <v>-2.0301410463246818</v>
+        <f t="shared" si="2"/>
+        <v>-2.1288891574357924</v>
       </c>
       <c r="H20">
         <f>(H9-H$2)-($B9-$B$2)</f>
@@ -1071,24 +1072,24 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <f>(C10-C$2)-($B10-$B$2)</f>
+        <f t="shared" si="1"/>
         <v>-1.5769999999999982</v>
       </c>
       <c r="D21">
-        <f>(D10-D$2)-($B10-$B$2)</f>
+        <f t="shared" si="1"/>
         <v>-0.37100000000000222</v>
       </c>
       <c r="E21">
-        <f>(E10-E$2)-($B10-$B$2)</f>
+        <f t="shared" si="1"/>
         <v>3.2929999999999993</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="0"/>
-        <v>5.5495256203419885</v>
+        <f t="shared" si="2"/>
+        <v>5.5618886203419891</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="0"/>
-        <v>2.122858953675324</v>
+        <f t="shared" si="2"/>
+        <v>2.0241108425642134</v>
       </c>
       <c r="H21">
         <f>(H10-H$2)-($B10-$B$2)</f>
@@ -1100,24 +1101,24 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <f>(C11-C$2)-($B11-$B$2)</f>
+        <f t="shared" si="1"/>
         <v>-0.28699999999999193</v>
       </c>
       <c r="D22">
-        <f>(D11-D$2)-($B11-$B$2)</f>
+        <f t="shared" si="1"/>
         <v>-3.2010000000000005</v>
       </c>
       <c r="E22">
-        <f>(E11-E$2)-($B11-$B$2)</f>
+        <f t="shared" si="1"/>
         <v>6.159000000000006</v>
       </c>
       <c r="F22" s="2">
-        <f t="shared" si="0"/>
-        <v>3.9085256203419831</v>
+        <f t="shared" si="2"/>
+        <v>3.9208886203419837</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="0"/>
-        <v>0.48185895367531872</v>
+        <f t="shared" si="2"/>
+        <v>0.3831108425642078</v>
       </c>
       <c r="H22">
         <f>(H11-H$2)-($B11-$B$2)</f>
@@ -1129,28 +1130,28 @@
         <v>31</v>
       </c>
       <c r="C23">
-        <f>(C12-C$2)-($B12-$B$2)</f>
-        <v>-2.0900915631131411</v>
+        <f t="shared" si="1"/>
+        <v>-2.2578206465067723</v>
       </c>
       <c r="D23">
-        <f>(D12-D$2)-($B12-$B$2)</f>
-        <v>-3.0648325210799072</v>
+        <f t="shared" si="1"/>
+        <v>-3.9557142857142793</v>
       </c>
       <c r="E23">
-        <f>(E12-E$2)-($B12-$B$2)</f>
-        <v>4.9348768018552178</v>
+        <f t="shared" si="1"/>
+        <v>6.7244382308083388</v>
       </c>
       <c r="F23">
         <f>(F12-F$2)-($B12-$B$2)</f>
-        <v>9.3085351293433334</v>
+        <v>6.1324620060790309</v>
       </c>
       <c r="G23">
         <f>(G12-G$2)-($B12-$B$2)</f>
-        <v>-5.4852299030340959</v>
+        <v>-4.3828571428571408</v>
       </c>
       <c r="H23" s="2">
         <f>F23*0.439183+G23*0.336042</f>
-        <v>2.2448827566350094</v>
+        <v>1.2204489812158077</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1158,72 +1159,72 @@
         <v>32</v>
       </c>
       <c r="C24">
-        <f>(C13-C$2)-($B13-$B$2)</f>
-        <v>-3.3863636363636402</v>
+        <f t="shared" si="1"/>
+        <v>-3.7211191335740068</v>
       </c>
       <c r="D24">
-        <f>(D13-D$2)-($B13-$B$2)</f>
-        <v>-6.1232326878897325</v>
+        <f t="shared" si="1"/>
+        <v>-5.5751242760304294</v>
       </c>
       <c r="E24">
-        <f>(E13-E$2)-($B13-$B$2)</f>
-        <v>11.476688785666887</v>
+        <f t="shared" si="1"/>
+        <v>8.7150541516245497</v>
       </c>
       <c r="F24">
         <f>(F13-F$2)-($B13-$B$2)</f>
-        <v>6.5107135874877784</v>
+        <v>11.969919348644289</v>
       </c>
       <c r="G24">
         <f>(G13-G$2)-($B13-$B$2)</f>
-        <v>-4.0503616813294272</v>
+        <v>-3.3269143278599387</v>
       </c>
       <c r="H24" s="2">
         <f>F24*0.439183+G24*0.336042</f>
-        <v>1.4983030853763413</v>
+        <v>4.1390021447329355</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C26">
         <f>AVERAGE(C16,C16,AVERAGE(C17,C18,C19),AVERAGE(C20,C21,C22),AVERAGE(C23,C24))</f>
-        <v>-0.56344551994767733</v>
+        <v>-0.54702731134141047</v>
       </c>
       <c r="D26">
-        <f t="shared" ref="D26:G26" si="1">AVERAGE(D16,D16,AVERAGE(D17,D18,D19),AVERAGE(D20,D21,D22),AVERAGE(D23,D24))</f>
-        <v>-2.2495398542302985</v>
+        <f t="shared" ref="D26:G26" si="3">AVERAGE(D16,D16,AVERAGE(D17,D18,D19),AVERAGE(D20,D21,D22),AVERAGE(D23,D24))</f>
+        <v>-2.3838171895078055</v>
       </c>
       <c r="E26">
-        <f t="shared" si="1"/>
-        <v>2.5934898920855423</v>
+        <f t="shared" si="3"/>
+        <v>2.4629492382432874</v>
       </c>
       <c r="F26">
-        <f t="shared" si="1"/>
-        <v>4.9175633290848388</v>
+        <f t="shared" si="3"/>
+        <v>5.081682526207393</v>
       </c>
       <c r="G26">
-        <f t="shared" si="1"/>
-        <v>-0.35925403436795611</v>
+        <f t="shared" si="3"/>
+        <v>-0.32975497855886715</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C27">
         <f>48.22+C26</f>
-        <v>47.656554480052321</v>
+        <v>47.672972688658589</v>
       </c>
       <c r="D27">
         <f>53.14+D26</f>
-        <v>50.890460145769701</v>
+        <v>50.756182810492191</v>
       </c>
       <c r="E27">
         <f>41.56+E26</f>
-        <v>44.153489892085545</v>
+        <v>44.022949238243292</v>
       </c>
       <c r="F27">
         <f>44.45+F26</f>
-        <v>49.367563329084845</v>
+        <v>49.531682526207398</v>
       </c>
       <c r="G27">
         <f>50.71+G26</f>
-        <v>50.350745965632044</v>
+        <v>50.380245021441134</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update for new polling
</commit_message>
<xml_diff>
--- a/Temporary Region Swings.xlsx
+++ b/Temporary Region Swings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BFCCD8-9762-456A-B9CF-E290850FAA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC74B0B-69D5-412D-A8D7-6EA1643A8AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="4455" windowWidth="24255" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="4110" windowWidth="20655" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
   <si>
     <t>NSW</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Second Essential (3 avg.) -&gt;</t>
+  </si>
+  <si>
+    <t>UAP</t>
   </si>
 </sst>
 </file>
@@ -478,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +493,7 @@
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -521,7 +524,7 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>48.47</v>
       </c>
@@ -556,37 +559,43 @@
         <v>16</v>
       </c>
       <c r="N2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" t="s">
         <v>17</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J3">
-        <v>46.18</v>
+        <v>33</v>
       </c>
       <c r="K3">
-        <v>30.94</v>
+        <v>35</v>
       </c>
       <c r="L3">
-        <v>14.08</v>
+        <v>10</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O3">
-        <v>8.8102400000000003</v>
+        <v>9</v>
       </c>
       <c r="P3">
-        <f>K3+L3*0.822+M3*0.348+(N3+O3)*(0.507)</f>
-        <v>46.980551680000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="Q3">
+        <f>K3+L3*0.822+M3*0.348+N3*0.352+(O3+P3)*(0.507)</f>
+        <v>53.277000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -612,7 +621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -646,34 +655,34 @@
       <c r="M5" t="s">
         <v>16</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>17</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
-        <v>57</v>
+        <v>56.5</v>
       </c>
       <c r="C6">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D6">
-        <v>57.5</v>
+        <v>63.5</v>
       </c>
       <c r="E6">
-        <v>51.5</v>
+        <v>48.5</v>
       </c>
       <c r="F6">
-        <v>53.5</v>
+        <v>52</v>
       </c>
       <c r="G6">
-        <v>59.5</v>
+        <v>52.5</v>
       </c>
       <c r="J6">
         <v>29.951599999999999</v>
@@ -687,18 +696,18 @@
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>0</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>27.469200000000001</v>
       </c>
-      <c r="P6">
-        <f>K6+L6*0.83+M6*0.348+(N6+O6)*(0.44)</f>
+      <c r="Q6">
+        <f>K6+L6*0.83+M6*0.348+(O6+P6)*(0.44)</f>
         <v>46.4633903</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -706,151 +715,151 @@
         <v>56.5</v>
       </c>
       <c r="C7">
-        <v>54</v>
+        <v>56.5</v>
       </c>
       <c r="D7">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E7">
-        <v>51.5</v>
+        <v>50</v>
       </c>
       <c r="F7">
-        <v>55.5</v>
+        <v>52</v>
       </c>
       <c r="G7">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>59.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C8">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D8">
-        <v>59</v>
+        <v>57.5</v>
       </c>
       <c r="E8">
-        <v>48.5</v>
+        <v>51.5</v>
       </c>
       <c r="F8">
-        <v>50.5</v>
+        <v>53.5</v>
       </c>
       <c r="G8">
-        <v>60.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <v>59.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
-        <v>53.704999999999998</v>
+        <v>53.277000000000001</v>
       </c>
       <c r="C9">
-        <v>52.332000000000001</v>
+        <v>53.266999999999996</v>
       </c>
       <c r="D9">
-        <v>58.515999999999998</v>
+        <v>53.224000000000004</v>
       </c>
       <c r="E9">
-        <v>48.938000000000002</v>
+        <v>52.902000000000001</v>
       </c>
       <c r="H9">
-        <v>54.055999999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>54.402999999999992</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10">
-        <v>49.183999999999997</v>
+        <v>53.704999999999998</v>
       </c>
       <c r="C10">
-        <v>47.356999999999999</v>
+        <v>52.332000000000001</v>
       </c>
       <c r="D10">
-        <v>53.482999999999997</v>
+        <v>58.515999999999998</v>
       </c>
       <c r="E10">
-        <v>45.567</v>
+        <v>48.938000000000002</v>
       </c>
       <c r="H10">
-        <v>53.688000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>54.055999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11">
-        <v>51.183999999999997</v>
+        <v>49.183999999999997</v>
       </c>
       <c r="C11">
-        <v>50.647000000000006</v>
+        <v>47.356999999999999</v>
       </c>
       <c r="D11">
-        <v>52.652999999999999</v>
+        <v>53.482999999999997</v>
       </c>
       <c r="E11">
-        <v>50.433000000000007</v>
+        <v>45.567</v>
       </c>
       <c r="H11">
-        <v>54.046999999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>53.688000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
       <c r="B12">
-        <v>52.142857142857139</v>
+        <v>51.785714285714285</v>
       </c>
       <c r="C12">
-        <v>49.635036496350367</v>
+        <v>50</v>
       </c>
       <c r="D12">
-        <v>52.857142857142861</v>
+        <v>50.533807829181498</v>
       </c>
       <c r="E12">
         <v>51.957295373665481</v>
       </c>
       <c r="F12">
-        <v>54.255319148936174</v>
+        <v>53.763440860215056</v>
       </c>
       <c r="G12">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>52.173913043478258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
       <c r="B13">
-        <v>51.624548736462089</v>
+        <v>52.346570397111911</v>
       </c>
       <c r="C13">
-        <v>47.653429602888082</v>
+        <v>49.637681159420282</v>
       </c>
       <c r="D13">
-        <v>50.719424460431661</v>
+        <v>53.81818181818182</v>
       </c>
       <c r="E13">
-        <v>53.429602888086642</v>
+        <v>50.183150183150175</v>
       </c>
       <c r="F13">
-        <v>59.574468085106382</v>
+        <v>61.05263157894737</v>
       </c>
       <c r="G13">
-        <v>50.537634408602152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>48.913043478260867</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -876,7 +885,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -916,41 +925,41 @@
       <c r="M16">
         <v>61.61</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>54.2</v>
       </c>
-      <c r="P16">
-        <f>(J16*J17+K16*K17+L16*L17+M16*M17+N16*N17)/SUM(J17:N17)</f>
+      <c r="Q16">
+        <f>(J16*J17+K16*K17+L16*L17+M16*M17+O16*O17)/SUM(J17:O17)</f>
         <v>49.554498799658013</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>2.25</v>
+        <v>-0.25</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>-4.1700000000000017</v>
+        <v>2.3299999999999983</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>1.4099999999999966</v>
+        <v>-1.0900000000000034</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>0.51999999999999602</v>
+        <v>-0.48000000000000398</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>0.25999999999999801</v>
+        <v>-6.240000000000002</v>
       </c>
       <c r="H17" s="2">
         <f>F17*0.439183+G17*0.336042</f>
-        <v>0.3157460799999976</v>
+        <v>-2.3077099200000024</v>
       </c>
       <c r="J17">
         <v>1401874</v>
@@ -964,48 +973,48 @@
       <c r="M17">
         <v>265975</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>103518</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>-2.25</v>
+        <v>0.25</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>-2.1700000000000017</v>
+        <v>-1.1700000000000017</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>1.9099999999999966</v>
+        <v>0.40999999999999659</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>3.019999999999996</v>
+        <v>-0.48000000000000398</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>5.259999999999998</v>
+        <v>0.75999999999999801</v>
       </c>
       <c r="H18" s="2">
         <f>F18*0.439183+G18*0.336042</f>
-        <v>3.0939135799999979</v>
+        <v>4.4584079999997583E-2</v>
       </c>
       <c r="J18">
-        <f>J17/SUM($J17:$N17)</f>
+        <f>J17/SUM($J17:$O17)</f>
         <v>0.43918262084011722</v>
       </c>
       <c r="K18">
-        <f>K17/SUM($J17:$N17)</f>
+        <f>K17/SUM($J17:$O17)</f>
         <v>0.3360418695823662</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1015,216 +1024,216 @@
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>-1.6700000000000017</v>
+        <v>-4.1700000000000017</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>-0.59000000000000341</v>
+        <v>1.4099999999999966</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>-1.480000000000004</v>
+        <v>0.51999999999999602</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>2.259999999999998</v>
+        <v>0.25999999999999801</v>
       </c>
       <c r="H19" s="2">
         <f>F19*0.439183+G19*0.336042</f>
-        <v>0.10946407999999763</v>
+        <v>0.3157460799999976</v>
       </c>
       <c r="L19">
-        <f>(J17+K17)/SUM(J17:N17)</f>
+        <f>(J17+K17)/SUM(J17:O17)</f>
         <v>0.77522449042248343</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="C20">
         <f t="shared" ref="C20:E24" si="1">(C9-C$2)-($B9-$B$2)</f>
-        <v>-1.1229999999999976</v>
+        <v>0.23999999999999488</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>0.14099999999999824</v>
+        <v>-4.722999999999999</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
-        <v>2.1430000000000007</v>
+        <v>6.5349999999999966</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" ref="F20:G22" si="2">AVERAGE(F$16,F$16,F$16,F$16,F$16,F$16,F$17,F$18,F$19)+($H20-AVERAGE($H$16,$H$16,$H$16,$H$16,$H$16,$H$16,$H$17,$H$18,$H$19))</f>
-        <v>1.4088886203419833</v>
+        <v>2.5135001203419751</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="2"/>
-        <v>-2.1288891574357924</v>
+        <v>-2.1909443241024675</v>
       </c>
       <c r="H20">
         <f>(H9-H$2)-($B9-$B$2)</f>
-        <v>-0.73349879965801534</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+        <v>4.150120034197613E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>-1.5769999999999982</v>
+        <v>-1.1229999999999976</v>
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
-        <v>-0.37100000000000222</v>
+        <v>0.14099999999999824</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
-        <v>3.2929999999999993</v>
+        <v>2.1430000000000007</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="2"/>
-        <v>5.5618886203419891</v>
+        <v>1.7385001203419836</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="2"/>
-        <v>2.0241108425642134</v>
+        <v>-2.965944324102459</v>
       </c>
       <c r="H21">
         <f>(H10-H$2)-($B10-$B$2)</f>
-        <v>3.4195012003419905</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+        <v>-0.73349879965801534</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>-0.28699999999999193</v>
+        <v>-1.5769999999999982</v>
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
-        <v>-3.2010000000000005</v>
+        <v>-0.37100000000000222</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
-        <v>6.159000000000006</v>
+        <v>3.2929999999999993</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="2"/>
-        <v>3.9208886203419837</v>
+        <v>5.8915001203419894</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="2"/>
-        <v>0.3831108425642078</v>
+        <v>1.1870556758975468</v>
       </c>
       <c r="H22">
         <f>(H11-H$2)-($B11-$B$2)</f>
-        <v>1.7785012003419851</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3.4195012003419905</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>-2.2578206465067723</v>
+        <v>-1.5357142857142847</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>-3.9557142857142793</v>
+        <v>-5.9219064565327884</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
-        <v>6.7244382308083388</v>
+        <v>7.0815810879511929</v>
       </c>
       <c r="F23">
         <f>(F12-F$2)-($B12-$B$2)</f>
-        <v>6.1324620060790309</v>
+        <v>5.9977265745007671</v>
       </c>
       <c r="G23">
         <f>(G12-G$2)-($B12-$B$2)</f>
-        <v>-4.3828571428571408</v>
+        <v>-1.8518012422360286</v>
       </c>
       <c r="H23" s="2">
         <f>F23*0.439183+G23*0.336042</f>
-        <v>1.2204489812158077</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+        <v>2.0118165571254907</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>-3.7211191335740068</v>
+        <v>-2.4588892376916291</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>-5.5751242760304294</v>
+        <v>-3.1983885789300928</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
-        <v>8.7150541516245497</v>
+        <v>4.7465797860382608</v>
       </c>
       <c r="F24">
         <f>(F13-F$2)-($B13-$B$2)</f>
-        <v>11.969919348644289</v>
+        <v>12.726061181835455</v>
       </c>
       <c r="G24">
         <f>(G13-G$2)-($B13-$B$2)</f>
-        <v>-3.3269143278599387</v>
+        <v>-5.6735269188510458</v>
       </c>
       <c r="H24" s="2">
         <f>F24*0.439183+G24*0.336042</f>
-        <v>4.1390021447329355</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3.6825263951574971</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C26">
         <f>AVERAGE(C16,C16,AVERAGE(C17,C18,C19),AVERAGE(C20,C21,C22),AVERAGE(C23,C24))</f>
-        <v>-0.54702731134141047</v>
+        <v>-0.31346035234059144</v>
       </c>
       <c r="D26">
         <f t="shared" ref="D26:G26" si="3">AVERAGE(D16,D16,AVERAGE(D17,D18,D19),AVERAGE(D20,D21,D22),AVERAGE(D23,D24))</f>
-        <v>-2.3838171895078055</v>
+        <v>-2.1108961702129561</v>
       </c>
       <c r="E26">
         <f t="shared" si="3"/>
-        <v>2.4629492382432874</v>
+        <v>1.9935494207322761</v>
       </c>
       <c r="F26">
         <f t="shared" si="3"/>
-        <v>5.081682526207393</v>
+        <v>4.927278799702016</v>
       </c>
       <c r="G26">
         <f t="shared" si="3"/>
-        <v>-0.32975497855886715</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+        <v>-1.4611883475958671</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C27">
         <f>48.22+C26</f>
-        <v>47.672972688658589</v>
+        <v>47.906539647659407</v>
       </c>
       <c r="D27">
         <f>53.14+D26</f>
-        <v>50.756182810492191</v>
+        <v>51.029103829787047</v>
       </c>
       <c r="E27">
         <f>41.56+E26</f>
-        <v>44.022949238243292</v>
+        <v>43.553549420732281</v>
       </c>
       <c r="F27">
         <f>44.45+F26</f>
-        <v>49.531682526207398</v>
+        <v>49.377278799702019</v>
       </c>
       <c r="G27">
         <f>50.71+G26</f>
-        <v>50.380245021441134</v>
+        <v>49.248811652404136</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add Morgan federal + SA YouGov polls
</commit_message>
<xml_diff>
--- a/Temporary Region Swings.xlsx
+++ b/Temporary Region Swings.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC74B0B-69D5-412D-A8D7-6EA1643A8AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B58D8A-3A27-4DC0-B607-99CC189F8AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="4110" windowWidth="20655" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22335" yWindow="3660" windowWidth="24255" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="1" r:id="rId1"/>
     <sheet name="Archives" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -483,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,22 +666,22 @@
         <v>8</v>
       </c>
       <c r="B6">
+        <v>56</v>
+      </c>
+      <c r="C6">
         <v>56.5</v>
       </c>
-      <c r="C6">
-        <v>56</v>
-      </c>
       <c r="D6">
-        <v>63.5</v>
+        <v>60</v>
       </c>
       <c r="E6">
-        <v>48.5</v>
+        <v>48</v>
       </c>
       <c r="F6">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G6">
-        <v>52.5</v>
+        <v>54.5</v>
       </c>
       <c r="J6">
         <v>29.951599999999999</v>
@@ -715,19 +714,19 @@
         <v>56.5</v>
       </c>
       <c r="C7">
-        <v>56.5</v>
+        <v>56</v>
       </c>
       <c r="D7">
-        <v>60</v>
+        <v>63.5</v>
       </c>
       <c r="E7">
-        <v>50</v>
+        <v>48.5</v>
       </c>
       <c r="F7">
         <v>52</v>
       </c>
       <c r="G7">
-        <v>59.5</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -735,19 +734,19 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>57</v>
+        <v>56.5</v>
       </c>
       <c r="C8">
-        <v>59</v>
+        <v>56.5</v>
       </c>
       <c r="D8">
-        <v>57.5</v>
+        <v>60</v>
       </c>
       <c r="E8">
-        <v>51.5</v>
+        <v>50</v>
       </c>
       <c r="F8">
-        <v>53.5</v>
+        <v>52</v>
       </c>
       <c r="G8">
         <v>59.5</v>
@@ -939,11 +938,11 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>-0.25</v>
+        <v>0.75</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>2.3299999999999983</v>
+        <v>-0.67000000000000171</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
@@ -951,15 +950,15 @@
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>-0.48000000000000398</v>
+        <v>1.019999999999996</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>-6.240000000000002</v>
+        <v>-3.740000000000002</v>
       </c>
       <c r="H17" s="2">
         <f>F17*0.439183+G17*0.336042</f>
-        <v>-2.3077099200000024</v>
+        <v>-0.80883042000000249</v>
       </c>
       <c r="J17">
         <v>1401874</v>
@@ -983,15 +982,15 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>-1.1700000000000017</v>
+        <v>2.3299999999999983</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>0.40999999999999659</v>
+        <v>-1.0900000000000034</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
@@ -999,11 +998,11 @@
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>0.75999999999999801</v>
+        <v>-6.240000000000002</v>
       </c>
       <c r="H18" s="2">
         <f>F18*0.439183+G18*0.336042</f>
-        <v>4.4584079999997583E-2</v>
+        <v>-2.3077099200000024</v>
       </c>
       <c r="J18">
         <f>J17/SUM($J17:$O17)</f>
@@ -1020,27 +1019,27 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>2.25</v>
+        <v>0.25</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>-4.1700000000000017</v>
+        <v>-1.1700000000000017</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>1.4099999999999966</v>
+        <v>0.40999999999999659</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>0.51999999999999602</v>
+        <v>-0.48000000000000398</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>0.25999999999999801</v>
+        <v>0.75999999999999801</v>
       </c>
       <c r="H19" s="2">
         <f>F19*0.439183+G19*0.336042</f>
-        <v>0.3157460799999976</v>
+        <v>4.4584079999997583E-2</v>
       </c>
       <c r="L19">
         <f>(J17+K17)/SUM(J17:O17)</f>
@@ -1065,11 +1064,11 @@
       </c>
       <c r="F20" s="2">
         <f t="shared" ref="F20:G22" si="2">AVERAGE(F$16,F$16,F$16,F$16,F$16,F$16,F$17,F$18,F$19)+($H20-AVERAGE($H$16,$H$16,$H$16,$H$16,$H$16,$H$16,$H$17,$H$18,$H$19))</f>
-        <v>2.5135001203419751</v>
+        <v>2.6940086203419749</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="2"/>
-        <v>-2.1909443241024675</v>
+        <v>-2.5104358241024674</v>
       </c>
       <c r="H20">
         <f>(H9-H$2)-($B9-$B$2)</f>
@@ -1094,11 +1093,11 @@
       </c>
       <c r="F21" s="2">
         <f t="shared" si="2"/>
-        <v>1.7385001203419836</v>
+        <v>1.9190086203419834</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="2"/>
-        <v>-2.965944324102459</v>
+        <v>-3.2854358241024588</v>
       </c>
       <c r="H21">
         <f>(H10-H$2)-($B10-$B$2)</f>
@@ -1123,11 +1122,11 @@
       </c>
       <c r="F22" s="2">
         <f t="shared" si="2"/>
-        <v>5.8915001203419894</v>
+        <v>6.0720086203419896</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="2"/>
-        <v>1.1870556758975468</v>
+        <v>0.86756417589754675</v>
       </c>
       <c r="H22">
         <f>(H11-H$2)-($B11-$B$2)</f>
@@ -1195,45 +1194,45 @@
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C26">
         <f>AVERAGE(C16,C16,AVERAGE(C17,C18,C19),AVERAGE(C20,C21,C22),AVERAGE(C23,C24))</f>
-        <v>-0.31346035234059144</v>
+        <v>-0.41346035234059142</v>
       </c>
       <c r="D26">
         <f t="shared" ref="D26:G26" si="3">AVERAGE(D16,D16,AVERAGE(D17,D18,D19),AVERAGE(D20,D21,D22),AVERAGE(D23,D24))</f>
-        <v>-2.1108961702129561</v>
+        <v>-1.8775628368796227</v>
       </c>
       <c r="E26">
         <f t="shared" si="3"/>
-        <v>1.9935494207322761</v>
+        <v>1.8268827540656098</v>
       </c>
       <c r="F26">
         <f t="shared" si="3"/>
-        <v>4.927278799702016</v>
+        <v>4.9967138330353489</v>
       </c>
       <c r="G26">
         <f t="shared" si="3"/>
-        <v>-1.4611883475958671</v>
+        <v>-1.7917533142625337</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C27">
         <f>48.22+C26</f>
-        <v>47.906539647659407</v>
+        <v>47.806539647659406</v>
       </c>
       <c r="D27">
         <f>53.14+D26</f>
-        <v>51.029103829787047</v>
+        <v>51.262437163120381</v>
       </c>
       <c r="E27">
         <f>41.56+E26</f>
-        <v>43.553549420732281</v>
+        <v>43.38688275406561</v>
       </c>
       <c r="F27">
         <f>44.45+F26</f>
-        <v>49.377278799702019</v>
+        <v>49.446713833035354</v>
       </c>
       <c r="G27">
         <f>50.71+G26</f>
-        <v>49.248811652404136</v>
+        <v>48.918246685737465</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add new poll and betting data.
</commit_message>
<xml_diff>
--- a/Temporary Region Swings.xlsx
+++ b/Temporary Region Swings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B58D8A-3A27-4DC0-B607-99CC189F8AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30559FC2-1F28-4E56-89C9-24431D375CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22335" yWindow="3660" windowWidth="24255" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19650" yWindow="4350" windowWidth="24255" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="1" r:id="rId1"/>
@@ -483,7 +483,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,22 +666,22 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C6">
-        <v>56.5</v>
+        <v>57.5</v>
       </c>
       <c r="D6">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E6">
-        <v>48</v>
+        <v>45.5</v>
       </c>
       <c r="F6">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G6">
-        <v>54.5</v>
+        <v>60.5</v>
       </c>
       <c r="J6">
         <v>29.951599999999999</v>
@@ -711,22 +711,22 @@
         <v>9</v>
       </c>
       <c r="B7">
+        <v>56</v>
+      </c>
+      <c r="C7">
         <v>56.5</v>
       </c>
-      <c r="C7">
-        <v>56</v>
-      </c>
       <c r="D7">
-        <v>63.5</v>
+        <v>60</v>
       </c>
       <c r="E7">
-        <v>48.5</v>
+        <v>48</v>
       </c>
       <c r="F7">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G7">
-        <v>52.5</v>
+        <v>54.5</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -737,19 +737,19 @@
         <v>56.5</v>
       </c>
       <c r="C8">
-        <v>56.5</v>
+        <v>56</v>
       </c>
       <c r="D8">
-        <v>60</v>
+        <v>63.5</v>
       </c>
       <c r="E8">
-        <v>50</v>
+        <v>48.5</v>
       </c>
       <c r="F8">
         <v>52</v>
       </c>
       <c r="G8">
-        <v>59.5</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -817,22 +817,22 @@
         <v>33</v>
       </c>
       <c r="B12">
-        <v>51.785714285714285</v>
+        <v>52.329749103942646</v>
       </c>
       <c r="C12">
-        <v>50</v>
+        <v>49.820788530465954</v>
       </c>
       <c r="D12">
-        <v>50.533807829181498</v>
+        <v>51.798561151079141</v>
       </c>
       <c r="E12">
         <v>51.957295373665481</v>
       </c>
       <c r="F12">
-        <v>53.763440860215056</v>
+        <v>54.838709677419352</v>
       </c>
       <c r="G12">
-        <v>52.173913043478258</v>
+        <v>54.255319148936174</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -840,19 +840,19 @@
         <v>34</v>
       </c>
       <c r="B13">
-        <v>52.346570397111911</v>
+        <v>52.158273381294968</v>
       </c>
       <c r="C13">
-        <v>49.637681159420282</v>
+        <v>49.81818181818182</v>
       </c>
       <c r="D13">
-        <v>53.81818181818182</v>
+        <v>53.763440860215056</v>
       </c>
       <c r="E13">
         <v>50.183150183150175</v>
       </c>
       <c r="F13">
-        <v>61.05263157894737</v>
+        <v>57.446808510638299</v>
       </c>
       <c r="G13">
         <v>48.913043478260867</v>
@@ -938,27 +938,27 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>-0.67000000000000171</v>
+        <v>1.3299999999999983</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>-1.0900000000000034</v>
+        <v>-5.5900000000000034</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>1.019999999999996</v>
+        <v>5.019999999999996</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>-3.740000000000002</v>
+        <v>0.25999999999999801</v>
       </c>
       <c r="H17" s="2">
         <f>F17*0.439183+G17*0.336042</f>
-        <v>-0.80883042000000249</v>
+        <v>2.2920695799999975</v>
       </c>
       <c r="J17">
         <v>1401874</v>
@@ -982,11 +982,11 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>-0.25</v>
+        <v>0.75</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>2.3299999999999983</v>
+        <v>-0.67000000000000171</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
@@ -994,15 +994,15 @@
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>-0.48000000000000398</v>
+        <v>1.019999999999996</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>-6.240000000000002</v>
+        <v>-3.740000000000002</v>
       </c>
       <c r="H18" s="2">
         <f>F18*0.439183+G18*0.336042</f>
-        <v>-2.3077099200000024</v>
+        <v>-0.80883042000000249</v>
       </c>
       <c r="J18">
         <f>J17/SUM($J17:$O17)</f>
@@ -1019,15 +1019,15 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>-1.1700000000000017</v>
+        <v>2.3299999999999983</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>0.40999999999999659</v>
+        <v>-1.0900000000000034</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
@@ -1035,11 +1035,11 @@
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>0.75999999999999801</v>
+        <v>-6.240000000000002</v>
       </c>
       <c r="H19" s="2">
         <f>F19*0.439183+G19*0.336042</f>
-        <v>4.4584079999997583E-2</v>
+        <v>-2.3077099200000024</v>
       </c>
       <c r="L19">
         <f>(J17+K17)/SUM(J17:O17)</f>
@@ -1064,11 +1064,11 @@
       </c>
       <c r="F20" s="2">
         <f t="shared" ref="F20:G22" si="2">AVERAGE(F$16,F$16,F$16,F$16,F$16,F$16,F$17,F$18,F$19)+($H20-AVERAGE($H$16,$H$16,$H$16,$H$16,$H$16,$H$16,$H$17,$H$18,$H$19))</f>
-        <v>2.6940086203419749</v>
+        <v>3.055399120341975</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="2"/>
-        <v>-2.5104358241024674</v>
+        <v>-2.8157119907691337</v>
       </c>
       <c r="H20">
         <f>(H9-H$2)-($B9-$B$2)</f>
@@ -1093,11 +1093,11 @@
       </c>
       <c r="F21" s="2">
         <f t="shared" si="2"/>
-        <v>1.9190086203419834</v>
+        <v>2.2803991203419836</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="2"/>
-        <v>-3.2854358241024588</v>
+        <v>-3.5907119907691252</v>
       </c>
       <c r="H21">
         <f>(H10-H$2)-($B10-$B$2)</f>
@@ -1122,11 +1122,11 @@
       </c>
       <c r="F22" s="2">
         <f t="shared" si="2"/>
-        <v>6.0720086203419896</v>
+        <v>6.4333991203419894</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="2"/>
-        <v>0.86756417589754675</v>
+        <v>0.5622880092308804</v>
       </c>
       <c r="H22">
         <f>(H11-H$2)-($B11-$B$2)</f>
@@ -1139,27 +1139,27 @@
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>-1.5357142857142847</v>
+        <v>-2.258960573476692</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>-5.9219064565327884</v>
+        <v>-5.2011879528635063</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
-        <v>7.0815810879511929</v>
+        <v>6.5375462697228315</v>
       </c>
       <c r="F23">
         <f>(F12-F$2)-($B12-$B$2)</f>
-        <v>5.9977265745007671</v>
+        <v>6.5289605734767022</v>
       </c>
       <c r="G23">
         <f>(G12-G$2)-($B12-$B$2)</f>
-        <v>-1.8518012422360286</v>
+        <v>-0.31442995500647442</v>
       </c>
       <c r="H23" s="2">
         <f>F23*0.439183+G23*0.336042</f>
-        <v>2.0118165571254907</v>
+        <v>2.761746820600933</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -1168,71 +1168,71 @@
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>-2.4588892376916291</v>
+        <v>-2.0900915631131483</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>-3.1983885789300928</v>
+        <v>-3.0648325210799143</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
-        <v>4.7465797860382608</v>
+        <v>4.9348768018552036</v>
       </c>
       <c r="F24">
         <f>(F13-F$2)-($B13-$B$2)</f>
-        <v>12.726061181835455</v>
+        <v>9.3085351293433263</v>
       </c>
       <c r="G24">
         <f>(G13-G$2)-($B13-$B$2)</f>
-        <v>-5.6735269188510458</v>
+        <v>-5.485229903034103</v>
       </c>
       <c r="H24" s="2">
         <f>F24*0.439183+G24*0.336042</f>
-        <v>3.6825263951574971</v>
+        <v>2.244882756635004</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C26">
         <f>AVERAGE(C16,C16,AVERAGE(C17,C18,C19),AVERAGE(C20,C21,C22),AVERAGE(C23,C24))</f>
-        <v>-0.41346035234059142</v>
+        <v>-0.48223854699231739</v>
       </c>
       <c r="D26">
         <f t="shared" ref="D26:G26" si="3">AVERAGE(D16,D16,AVERAGE(D17,D18,D19),AVERAGE(D20,D21,D22),AVERAGE(D23,D24))</f>
-        <v>-1.8775628368796227</v>
+        <v>-1.6254687140610102</v>
       </c>
       <c r="E26">
         <f t="shared" si="3"/>
-        <v>1.8268827540656098</v>
+        <v>1.3913089738244679</v>
       </c>
       <c r="F26">
         <f t="shared" si="3"/>
-        <v>4.9967138330353489</v>
+        <v>5.1470293943503966</v>
       </c>
       <c r="G26">
         <f t="shared" si="3"/>
-        <v>-1.7917533142625337</v>
+        <v>-1.7135750506245508</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C27">
         <f>48.22+C26</f>
-        <v>47.806539647659406</v>
+        <v>47.737761453007678</v>
       </c>
       <c r="D27">
         <f>53.14+D26</f>
-        <v>51.262437163120381</v>
+        <v>51.514531285938993</v>
       </c>
       <c r="E27">
         <f>41.56+E26</f>
-        <v>43.38688275406561</v>
+        <v>42.951308973824467</v>
       </c>
       <c r="F27">
         <f>44.45+F26</f>
-        <v>49.446713833035354</v>
+        <v>49.5970293943504</v>
       </c>
       <c r="G27">
         <f>50.71+G26</f>
-        <v>48.918246685737465</v>
+        <v>48.996424949375452</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Enter and save Tcp changes.
</commit_message>
<xml_diff>
--- a/Temporary Region Swings.xlsx
+++ b/Temporary Region Swings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30559FC2-1F28-4E56-89C9-24431D375CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54390B83-61E4-4CD0-BD87-A0666D41F02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19650" yWindow="4350" windowWidth="24255" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18150" yWindow="4695" windowWidth="24255" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="1" r:id="rId1"/>
@@ -483,7 +483,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,22 +625,22 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C5">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D5">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E5">
         <v>46</v>
       </c>
       <c r="F5">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G5">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J5" t="s">
         <v>13</v>
@@ -890,7 +890,7 @@
       </c>
       <c r="C16">
         <f t="shared" ref="C16:G19" si="0">(C5-C$2)-($B5-$B$2)</f>
-        <v>0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
@@ -898,19 +898,19 @@
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>-9.0000000000003411E-2</v>
+        <v>-2.0900000000000034</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>6.019999999999996</v>
+        <v>2.019999999999996</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>-0.24000000000000199</v>
+        <v>1.759999999999998</v>
       </c>
       <c r="H16" s="2">
         <f>F16*0.439183+G16*0.336042</f>
-        <v>2.5632315799999974</v>
+        <v>1.4785835799999978</v>
       </c>
       <c r="J16">
         <v>44.45</v>
@@ -1064,11 +1064,11 @@
       </c>
       <c r="F20" s="2">
         <f t="shared" ref="F20:G22" si="2">AVERAGE(F$16,F$16,F$16,F$16,F$16,F$16,F$17,F$18,F$19)+($H20-AVERAGE($H$16,$H$16,$H$16,$H$16,$H$16,$H$16,$H$17,$H$18,$H$19))</f>
-        <v>3.055399120341975</v>
+        <v>1.1118311203419744</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="2"/>
-        <v>-2.8157119907691337</v>
+        <v>-0.75927999076913466</v>
       </c>
       <c r="H20">
         <f>(H9-H$2)-($B9-$B$2)</f>
@@ -1093,11 +1093,11 @@
       </c>
       <c r="F21" s="2">
         <f t="shared" si="2"/>
-        <v>2.2803991203419836</v>
+        <v>0.33683112034198293</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="2"/>
-        <v>-3.5907119907691252</v>
+        <v>-1.5342799907691262</v>
       </c>
       <c r="H21">
         <f>(H10-H$2)-($B10-$B$2)</f>
@@ -1122,11 +1122,11 @@
       </c>
       <c r="F22" s="2">
         <f t="shared" si="2"/>
-        <v>6.4333991203419894</v>
+        <v>4.4898311203419885</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="2"/>
-        <v>0.5622880092308804</v>
+        <v>2.6187200092308798</v>
       </c>
       <c r="H22">
         <f>(H11-H$2)-($B11-$B$2)</f>
@@ -1194,7 +1194,7 @@
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C26">
         <f>AVERAGE(C16,C16,AVERAGE(C17,C18,C19),AVERAGE(C20,C21,C22),AVERAGE(C23,C24))</f>
-        <v>-0.48223854699231739</v>
+        <v>-0.88223854699231752</v>
       </c>
       <c r="D26">
         <f t="shared" ref="D26:G26" si="3">AVERAGE(D16,D16,AVERAGE(D17,D18,D19),AVERAGE(D20,D21,D22),AVERAGE(D23,D24))</f>
@@ -1202,21 +1202,21 @@
       </c>
       <c r="E26">
         <f t="shared" si="3"/>
-        <v>1.3913089738244679</v>
+        <v>0.5913089738244679</v>
       </c>
       <c r="F26">
         <f t="shared" si="3"/>
-        <v>5.1470293943503966</v>
+        <v>3.158315794350397</v>
       </c>
       <c r="G26">
         <f t="shared" si="3"/>
-        <v>-1.7135750506245508</v>
+        <v>-0.50228865062455097</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C27">
         <f>48.22+C26</f>
-        <v>47.737761453007678</v>
+        <v>47.33776145300768</v>
       </c>
       <c r="D27">
         <f>53.14+D26</f>
@@ -1224,15 +1224,15 @@
       </c>
       <c r="E27">
         <f>41.56+E26</f>
-        <v>42.951308973824467</v>
+        <v>42.15130897382447</v>
       </c>
       <c r="F27">
         <f>44.45+F26</f>
-        <v>49.5970293943504</v>
+        <v>47.608315794350403</v>
       </c>
       <c r="G27">
         <f>50.71+G26</f>
-        <v>48.996424949375452</v>
+        <v>50.207711349375451</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update for latest Morgan poll
</commit_message>
<xml_diff>
--- a/Temporary Region Swings.xlsx
+++ b/Temporary Region Swings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54390B83-61E4-4CD0-BD87-A0666D41F02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3870DAD-3EE6-4647-86FF-F7AF1EA17396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18150" yWindow="4695" windowWidth="24255" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="3780" windowWidth="24255" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="1" r:id="rId1"/>
@@ -483,7 +483,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,22 +666,22 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>58</v>
+        <v>55.5</v>
       </c>
       <c r="C6">
-        <v>57.5</v>
+        <v>53</v>
       </c>
       <c r="D6">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E6">
-        <v>45.5</v>
+        <v>49</v>
       </c>
       <c r="F6">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G6">
-        <v>60.5</v>
+        <v>63.5</v>
       </c>
       <c r="J6">
         <v>29.951599999999999</v>
@@ -711,22 +711,22 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C7">
-        <v>56.5</v>
+        <v>57.5</v>
       </c>
       <c r="D7">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E7">
-        <v>48</v>
+        <v>45.5</v>
       </c>
       <c r="F7">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G7">
-        <v>54.5</v>
+        <v>60.5</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -734,22 +734,22 @@
         <v>10</v>
       </c>
       <c r="B8">
+        <v>56</v>
+      </c>
+      <c r="C8">
         <v>56.5</v>
       </c>
-      <c r="C8">
-        <v>56</v>
-      </c>
       <c r="D8">
-        <v>63.5</v>
+        <v>60</v>
       </c>
       <c r="E8">
-        <v>48.5</v>
+        <v>48</v>
       </c>
       <c r="F8">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G8">
-        <v>52.5</v>
+        <v>54.5</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -938,27 +938,27 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>-0.25</v>
+        <v>-2.25</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>1.3299999999999983</v>
+        <v>-0.17000000000000171</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>-5.5900000000000034</v>
+        <v>0.40999999999999659</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>5.019999999999996</v>
+        <v>5.519999999999996</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>0.25999999999999801</v>
+        <v>5.759999999999998</v>
       </c>
       <c r="H17" s="2">
         <f>F17*0.439183+G17*0.336042</f>
-        <v>2.2920695799999975</v>
+        <v>4.3598920799999981</v>
       </c>
       <c r="J17">
         <v>1401874</v>
@@ -982,27 +982,27 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>-0.67000000000000171</v>
+        <v>1.3299999999999983</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>-1.0900000000000034</v>
+        <v>-5.5900000000000034</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>1.019999999999996</v>
+        <v>5.019999999999996</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>-3.740000000000002</v>
+        <v>0.25999999999999801</v>
       </c>
       <c r="H18" s="2">
         <f>F18*0.439183+G18*0.336042</f>
-        <v>-0.80883042000000249</v>
+        <v>2.2920695799999975</v>
       </c>
       <c r="J18">
         <f>J17/SUM($J17:$O17)</f>
@@ -1019,11 +1019,11 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>-0.25</v>
+        <v>0.75</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>2.3299999999999983</v>
+        <v>-0.67000000000000171</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
@@ -1031,15 +1031,15 @@
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>-0.48000000000000398</v>
+        <v>1.019999999999996</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>-6.240000000000002</v>
+        <v>-3.740000000000002</v>
       </c>
       <c r="H19" s="2">
         <f>F19*0.439183+G19*0.336042</f>
-        <v>-2.3077099200000024</v>
+        <v>-0.80883042000000249</v>
       </c>
       <c r="L19">
         <f>(J17+K17)/SUM(J17:O17)</f>
@@ -1064,11 +1064,11 @@
       </c>
       <c r="F20" s="2">
         <f t="shared" ref="F20:G22" si="2">AVERAGE(F$16,F$16,F$16,F$16,F$16,F$16,F$17,F$18,F$19)+($H20-AVERAGE($H$16,$H$16,$H$16,$H$16,$H$16,$H$16,$H$17,$H$18,$H$19))</f>
-        <v>1.1118311203419744</v>
+        <v>1.0376531203419745</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="2"/>
-        <v>-0.75927999076913466</v>
+        <v>-0.16679132410246789</v>
       </c>
       <c r="H20">
         <f>(H9-H$2)-($B9-$B$2)</f>
@@ -1093,11 +1093,11 @@
       </c>
       <c r="F21" s="2">
         <f t="shared" si="2"/>
-        <v>0.33683112034198293</v>
+        <v>0.26265312034198329</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="2"/>
-        <v>-1.5342799907691262</v>
+        <v>-0.94179132410245914</v>
       </c>
       <c r="H21">
         <f>(H10-H$2)-($B10-$B$2)</f>
@@ -1122,11 +1122,11 @@
       </c>
       <c r="F22" s="2">
         <f t="shared" si="2"/>
-        <v>4.4898311203419885</v>
+        <v>4.4156531203419886</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="2"/>
-        <v>2.6187200092308798</v>
+        <v>3.2112086758975464</v>
       </c>
       <c r="H22">
         <f>(H11-H$2)-($B11-$B$2)</f>
@@ -1194,45 +1194,45 @@
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C26">
         <f>AVERAGE(C16,C16,AVERAGE(C17,C18,C19),AVERAGE(C20,C21,C22),AVERAGE(C23,C24))</f>
-        <v>-0.88223854699231752</v>
+        <v>-1.0155718803256508</v>
       </c>
       <c r="D26">
         <f t="shared" ref="D26:G26" si="3">AVERAGE(D16,D16,AVERAGE(D17,D18,D19),AVERAGE(D20,D21,D22),AVERAGE(D23,D24))</f>
-        <v>-1.6254687140610102</v>
+        <v>-1.7921353807276765</v>
       </c>
       <c r="E26">
         <f t="shared" si="3"/>
-        <v>0.5913089738244679</v>
+        <v>0.69130897382446788</v>
       </c>
       <c r="F26">
         <f t="shared" si="3"/>
-        <v>3.158315794350397</v>
+        <v>3.5434801943503969</v>
       </c>
       <c r="G26">
         <f t="shared" si="3"/>
-        <v>-0.50228865062455097</v>
+        <v>0.41620908270878232</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C27">
         <f>48.22+C26</f>
-        <v>47.33776145300768</v>
+        <v>47.204428119674347</v>
       </c>
       <c r="D27">
         <f>53.14+D26</f>
-        <v>51.514531285938993</v>
+        <v>51.347864619272322</v>
       </c>
       <c r="E27">
         <f>41.56+E26</f>
-        <v>42.15130897382447</v>
+        <v>42.251308973824472</v>
       </c>
       <c r="F27">
         <f>44.45+F26</f>
-        <v>47.608315794350403</v>
+        <v>47.993480194350397</v>
       </c>
       <c r="G27">
         <f>50.71+G26</f>
-        <v>50.207711349375451</v>
+        <v>51.126209082708783</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update with new polls.
</commit_message>
<xml_diff>
--- a/Temporary Region Swings.xlsx
+++ b/Temporary Region Swings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3870DAD-3EE6-4647-86FF-F7AF1EA17396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF79D0EA-ABF6-4F47-8734-76DD039E958A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="3780" windowWidth="24255" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="3780" windowWidth="24255" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="1" r:id="rId1"/>
@@ -483,7 +483,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I20" sqref="I20:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,29 +569,29 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J3">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K3">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="L3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M3">
         <v>3</v>
       </c>
       <c r="N3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="Q3">
         <f>K3+L3*0.822+M3*0.348+N3*0.352+(O3+P3)*(0.507)</f>
-        <v>53.277000000000001</v>
+        <v>60.86399999999999</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -666,22 +666,22 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>55.5</v>
+        <v>57</v>
       </c>
       <c r="C6">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D6">
-        <v>60</v>
+        <v>60.5</v>
       </c>
       <c r="E6">
-        <v>49</v>
+        <v>50.5</v>
       </c>
       <c r="F6">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G6">
-        <v>63.5</v>
+        <v>56</v>
       </c>
       <c r="J6">
         <v>29.951599999999999</v>
@@ -711,22 +711,22 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>58</v>
+        <v>55.5</v>
       </c>
       <c r="C7">
-        <v>57.5</v>
+        <v>53</v>
       </c>
       <c r="D7">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E7">
-        <v>45.5</v>
+        <v>49</v>
       </c>
       <c r="F7">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G7">
-        <v>60.5</v>
+        <v>63.5</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -734,22 +734,22 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C8">
-        <v>56.5</v>
+        <v>57.5</v>
       </c>
       <c r="D8">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E8">
-        <v>48</v>
+        <v>45.5</v>
       </c>
       <c r="F8">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G8">
-        <v>54.5</v>
+        <v>60.5</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -757,19 +757,19 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>53.277000000000001</v>
+        <v>54.878</v>
       </c>
       <c r="C9">
-        <v>53.266999999999996</v>
+        <v>52.726999999999997</v>
       </c>
       <c r="D9">
-        <v>53.224000000000004</v>
+        <v>53.233999999999995</v>
       </c>
       <c r="E9">
-        <v>52.902000000000001</v>
+        <v>53.542999999999999</v>
       </c>
       <c r="H9">
-        <v>54.402999999999992</v>
+        <v>60.86399999999999</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -777,19 +777,19 @@
         <v>19</v>
       </c>
       <c r="B10">
-        <v>53.704999999999998</v>
+        <v>53.277000000000001</v>
       </c>
       <c r="C10">
-        <v>52.332000000000001</v>
+        <v>53.266999999999996</v>
       </c>
       <c r="D10">
-        <v>58.515999999999998</v>
+        <v>53.224000000000004</v>
       </c>
       <c r="E10">
-        <v>48.938000000000002</v>
+        <v>52.902000000000001</v>
       </c>
       <c r="H10">
-        <v>54.055999999999997</v>
+        <v>54.402999999999992</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -797,19 +797,19 @@
         <v>20</v>
       </c>
       <c r="B11">
-        <v>49.183999999999997</v>
+        <v>53.704999999999998</v>
       </c>
       <c r="C11">
-        <v>47.356999999999999</v>
+        <v>52.332000000000001</v>
       </c>
       <c r="D11">
-        <v>53.482999999999997</v>
+        <v>58.515999999999998</v>
       </c>
       <c r="E11">
-        <v>45.567</v>
+        <v>48.938000000000002</v>
       </c>
       <c r="H11">
-        <v>53.688000000000002</v>
+        <v>54.055999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -817,22 +817,22 @@
         <v>33</v>
       </c>
       <c r="B12">
-        <v>52.329749103942646</v>
+        <v>52.499999999999993</v>
       </c>
       <c r="C12">
-        <v>49.820788530465954</v>
+        <v>51.236749116607776</v>
       </c>
       <c r="D12">
-        <v>51.798561151079141</v>
+        <v>51.27272727272728</v>
       </c>
       <c r="E12">
-        <v>51.957295373665481</v>
+        <v>52.158273381294968</v>
       </c>
       <c r="F12">
-        <v>54.838709677419352</v>
+        <v>53.191489361702125</v>
       </c>
       <c r="G12">
-        <v>54.255319148936174</v>
+        <v>52.631578947368418</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -840,22 +840,22 @@
         <v>34</v>
       </c>
       <c r="B13">
-        <v>52.158273381294968</v>
+        <v>52.142857142857139</v>
       </c>
       <c r="C13">
-        <v>49.81818181818182</v>
+        <v>49.635036496350367</v>
       </c>
       <c r="D13">
-        <v>53.763440860215056</v>
+        <v>52.857142857142861</v>
       </c>
       <c r="E13">
-        <v>50.183150183150175</v>
+        <v>51.957295373665481</v>
       </c>
       <c r="F13">
-        <v>57.446808510638299</v>
+        <v>54.255319148936174</v>
       </c>
       <c r="G13">
-        <v>48.913043478260867</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -938,11 +938,11 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>-2.25</v>
+        <v>-1.75</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>-0.17000000000000171</v>
+        <v>-1.1700000000000017</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
@@ -950,15 +950,15 @@
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>5.519999999999996</v>
+        <v>6.019999999999996</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>5.759999999999998</v>
+        <v>-3.240000000000002</v>
       </c>
       <c r="H17" s="2">
         <f>F17*0.439183+G17*0.336042</f>
-        <v>4.3598920799999981</v>
+        <v>1.5551055799999975</v>
       </c>
       <c r="J17">
         <v>1401874</v>
@@ -982,27 +982,27 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>-0.25</v>
+        <v>-2.25</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>1.3299999999999983</v>
+        <v>-0.17000000000000171</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>-5.5900000000000034</v>
+        <v>0.40999999999999659</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>5.019999999999996</v>
+        <v>5.519999999999996</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>0.25999999999999801</v>
+        <v>5.759999999999998</v>
       </c>
       <c r="H18" s="2">
         <f>F18*0.439183+G18*0.336042</f>
-        <v>2.2920695799999975</v>
+        <v>4.3598920799999981</v>
       </c>
       <c r="J18">
         <f>J17/SUM($J17:$O17)</f>
@@ -1019,27 +1019,27 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>-0.67000000000000171</v>
+        <v>1.3299999999999983</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>-1.0900000000000034</v>
+        <v>-5.5900000000000034</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>1.019999999999996</v>
+        <v>5.019999999999996</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>-3.740000000000002</v>
+        <v>0.25999999999999801</v>
       </c>
       <c r="H19" s="2">
         <f>F19*0.439183+G19*0.336042</f>
-        <v>-0.80883042000000249</v>
+        <v>2.2920695799999975</v>
       </c>
       <c r="L19">
         <f>(J17+K17)/SUM(J17:O17)</f>
@@ -1052,27 +1052,27 @@
       </c>
       <c r="C20">
         <f t="shared" ref="C20:E24" si="1">(C9-C$2)-($B9-$B$2)</f>
-        <v>0.23999999999999488</v>
+        <v>-1.9010000000000034</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>-4.722999999999999</v>
+        <v>-6.3140000000000072</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
-        <v>6.5349999999999966</v>
+        <v>5.5749999999999957</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" ref="F20:G22" si="2">AVERAGE(F$16,F$16,F$16,F$16,F$16,F$16,F$17,F$18,F$19)+($H20-AVERAGE($H$16,$H$16,$H$16,$H$16,$H$16,$H$16,$H$17,$H$18,$H$19))</f>
-        <v>1.0376531203419745</v>
+        <v>6.1905491203419736</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="2"/>
-        <v>-0.16679132410246789</v>
+        <v>4.4861046758975318</v>
       </c>
       <c r="H20">
         <f>(H9-H$2)-($B9-$B$2)</f>
-        <v>4.150120034197613E-2</v>
+        <v>4.9015012003419756</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1081,27 +1081,27 @@
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>-1.1229999999999976</v>
+        <v>0.23999999999999488</v>
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
-        <v>0.14099999999999824</v>
+        <v>-4.722999999999999</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
-        <v>2.1430000000000007</v>
+        <v>6.5349999999999966</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="2"/>
-        <v>0.26265312034198329</v>
+        <v>1.3305491203419744</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="2"/>
-        <v>-0.94179132410245914</v>
+        <v>-0.37389532410246784</v>
       </c>
       <c r="H21">
         <f>(H10-H$2)-($B10-$B$2)</f>
-        <v>-0.73349879965801534</v>
+        <v>4.150120034197613E-2</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1110,27 +1110,27 @@
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>-1.5769999999999982</v>
+        <v>-1.1229999999999976</v>
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
-        <v>-0.37100000000000222</v>
+        <v>0.14099999999999824</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
-        <v>3.2929999999999993</v>
+        <v>2.1430000000000007</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="2"/>
-        <v>4.4156531203419886</v>
+        <v>0.55554912034198312</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="2"/>
-        <v>3.2112086758975464</v>
+        <v>-1.1488953241024591</v>
       </c>
       <c r="H22">
         <f>(H11-H$2)-($B11-$B$2)</f>
-        <v>3.4195012003419905</v>
+        <v>-0.73349879965801534</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -1139,27 +1139,27 @@
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>-2.258960573476692</v>
+        <v>-1.0132508833922174</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>-5.2011879528635063</v>
+        <v>-5.8972727272727141</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
-        <v>6.5375462697228315</v>
+        <v>6.5682733812949721</v>
       </c>
       <c r="F23">
         <f>(F12-F$2)-($B12-$B$2)</f>
-        <v>6.5289605734767022</v>
+        <v>4.7114893617021281</v>
       </c>
       <c r="G23">
         <f>(G12-G$2)-($B12-$B$2)</f>
-        <v>-0.31442995500647442</v>
+        <v>-2.1084210526315772</v>
       </c>
       <c r="H23" s="2">
         <f>F23*0.439183+G23*0.336042</f>
-        <v>2.761746820600933</v>
+        <v>1.3606880049720051</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -1168,71 +1168,71 @@
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>-2.0900915631131483</v>
+        <v>-2.2578206465067723</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>-3.0648325210799143</v>
+        <v>-3.9557142857142793</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
-        <v>4.9348768018552036</v>
+        <v>6.7244382308083388</v>
       </c>
       <c r="F24">
         <f>(F13-F$2)-($B13-$B$2)</f>
-        <v>9.3085351293433263</v>
+        <v>6.1324620060790309</v>
       </c>
       <c r="G24">
         <f>(G13-G$2)-($B13-$B$2)</f>
-        <v>-5.485229903034103</v>
+        <v>-4.3828571428571408</v>
       </c>
       <c r="H24" s="2">
         <f>F24*0.439183+G24*0.336042</f>
-        <v>2.244882756635004</v>
+        <v>1.2204489812158077</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C26">
         <f>AVERAGE(C16,C16,AVERAGE(C17,C18,C19),AVERAGE(C20,C21,C22),AVERAGE(C23,C24))</f>
-        <v>-1.0155718803256508</v>
+        <v>-1.0960404863232327</v>
       </c>
       <c r="D26">
         <f t="shared" ref="D26:G26" si="3">AVERAGE(D16,D16,AVERAGE(D17,D18,D19),AVERAGE(D20,D21,D22),AVERAGE(D23,D24))</f>
-        <v>-1.7921353807276765</v>
+        <v>-2.3803653679653678</v>
       </c>
       <c r="E26">
         <f t="shared" si="3"/>
-        <v>0.69130897382446788</v>
+        <v>1.1254711612103285</v>
       </c>
       <c r="F26">
         <f t="shared" si="3"/>
-        <v>3.5434801943503969</v>
+        <v>3.534838294179842</v>
       </c>
       <c r="G26">
         <f t="shared" si="3"/>
-        <v>0.41620908270878232</v>
+        <v>0.43775978229730067</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C27">
         <f>48.22+C26</f>
-        <v>47.204428119674347</v>
+        <v>47.123959513676766</v>
       </c>
       <c r="D27">
         <f>53.14+D26</f>
-        <v>51.347864619272322</v>
+        <v>50.759634632034633</v>
       </c>
       <c r="E27">
         <f>41.56+E26</f>
-        <v>42.251308973824472</v>
+        <v>42.68547116121033</v>
       </c>
       <c r="F27">
         <f>44.45+F26</f>
-        <v>47.993480194350397</v>
+        <v>47.984838294179845</v>
       </c>
       <c r="G27">
         <f>50.71+G26</f>
-        <v>51.126209082708783</v>
+        <v>51.1477597822973</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update with latest polling
</commit_message>
<xml_diff>
--- a/Temporary Region Swings.xlsx
+++ b/Temporary Region Swings.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2C0DA0-DCF2-403D-8D10-FCE7147836D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{043361D8-F416-48A5-B398-16B88CDAAB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="4995" windowWidth="27960" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16185" yWindow="4845" windowWidth="27960" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="1" r:id="rId1"/>
     <sheet name="Archives" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -486,7 +487,7 @@
   <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="I26" sqref="I26:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,22 +670,22 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>54.5</v>
+        <v>55.5</v>
       </c>
       <c r="C6">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D6">
-        <v>60</v>
+        <v>63.5</v>
       </c>
       <c r="E6">
-        <v>45.5</v>
+        <v>43.5</v>
       </c>
       <c r="F6">
-        <v>45.5</v>
+        <v>49</v>
       </c>
       <c r="G6">
-        <v>61.5</v>
+        <v>62.5</v>
       </c>
       <c r="J6">
         <v>29.951599999999999</v>
@@ -714,22 +715,22 @@
         <v>9</v>
       </c>
       <c r="B7">
+        <v>54.5</v>
+      </c>
+      <c r="C7">
         <v>55</v>
       </c>
-      <c r="C7">
-        <v>53.5</v>
-      </c>
       <c r="D7">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E7">
-        <v>51.5</v>
+        <v>45.5</v>
       </c>
       <c r="F7">
-        <v>49</v>
+        <v>45.5</v>
       </c>
       <c r="G7">
-        <v>58</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -737,22 +738,22 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C8">
-        <v>55</v>
+        <v>53.5</v>
       </c>
       <c r="D8">
         <v>58</v>
       </c>
       <c r="E8">
-        <v>50.5</v>
+        <v>51.5</v>
       </c>
       <c r="F8">
-        <v>63.5</v>
+        <v>49</v>
       </c>
       <c r="G8">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -968,15 +969,15 @@
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>0.82999999999999829</v>
+        <v>3.3299999999999983</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>-2.0900000000000034</v>
+        <v>-5.0900000000000034</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>-4.980000000000004</v>
+        <v>-2.480000000000004</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
@@ -984,7 +985,7 @@
       </c>
       <c r="H18" s="2">
         <f>F18*0.439183+G18*0.336042</f>
-        <v>-0.5875714200000024</v>
+        <v>0.51038607999999774</v>
       </c>
       <c r="J18">
         <v>1401874</v>
@@ -1008,27 +1009,27 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>-1.25</v>
+        <v>0.75</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>-1.6700000000000017</v>
+        <v>0.82999999999999829</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>3.4099999999999966</v>
+        <v>-2.0900000000000034</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>-1.980000000000004</v>
+        <v>-4.980000000000004</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>0.75999999999999801</v>
+        <v>4.759999999999998</v>
       </c>
       <c r="H19" s="2">
         <f>F19*0.439183+G19*0.336042</f>
-        <v>-0.61419042000000235</v>
+        <v>-0.5875714200000024</v>
       </c>
       <c r="J19">
         <f>J18/SUM($J18:$O18)</f>
@@ -1045,27 +1046,27 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>-1.75</v>
+        <v>-1.25</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>-3.6700000000000017</v>
+        <v>-1.6700000000000017</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>0.40999999999999659</v>
+        <v>3.4099999999999966</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>10.519999999999996</v>
+        <v>-1.980000000000004</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
-        <v>-6.240000000000002</v>
+        <v>0.75999999999999801</v>
       </c>
       <c r="H20" s="2">
         <f>F20*0.439183+G20*0.336042</f>
-        <v>2.5233030799999976</v>
+        <v>-0.61419042000000235</v>
       </c>
       <c r="L20">
         <f>(J18+K18)/SUM(J18:O18)</f>
@@ -1090,11 +1091,11 @@
       </c>
       <c r="F21" s="2">
         <f t="shared" ref="F21:G23" si="2">AVERAGE(F$17,F$17,F$17,F$17,F$17,F$17,F$18,F$19,F$20)+($H21-AVERAGE($H$17,$H$17,$H$17,$H$17,$H$17,$H$17,$H$18,$H$19,$H$20))</f>
-        <v>-1.2928368796580139</v>
+        <v>-2.5136238796580139</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="2"/>
-        <v>-1.9417257685469009</v>
+        <v>-0.49584610188023426</v>
       </c>
       <c r="H21">
         <f>(H9-H$2)-($B9-$B$2)</f>
@@ -1119,11 +1120,11 @@
       </c>
       <c r="F22" s="2">
         <f t="shared" si="2"/>
-        <v>0.65116312034197454</v>
+        <v>-0.56962387965802563</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="2"/>
-        <v>2.2742314530874719E-3</v>
+        <v>1.4481538981197539</v>
       </c>
       <c r="H22">
         <f>(H10-H$2)-($B10-$B$2)</f>
@@ -1148,11 +1149,11 @@
       </c>
       <c r="F23" s="2">
         <f t="shared" si="2"/>
-        <v>5.5111631203419744</v>
+        <v>4.2903761203419739</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="2"/>
-        <v>4.8622742314530871</v>
+        <v>6.3081538981197536</v>
       </c>
       <c r="H23">
         <f>(H11-H$2)-($B11-$B$2)</f>
@@ -1249,45 +1250,45 @@
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C28">
         <f>AVERAGE(C17,C17,AVERAGE(C18,C19,C20),AVERAGE(C21,C22,C23),AVERAGE(C24,C25),AVERAGE(C26,C17,C17,AVERAGE(C18,C19,C20),AVERAGE(C21,C22,C23),AVERAGE(C24,C25),C17,C17,AVERAGE(C18,C19,C20),AVERAGE(C21,C22,C23),AVERAGE(C24,C25)))</f>
-        <v>-0.65693172120591536</v>
+        <v>-0.49279030706450122</v>
       </c>
       <c r="D28">
-        <f t="shared" ref="D28:G28" si="4">AVERAGE(D17,D17,AVERAGE(D18,D19,D20),AVERAGE(D21,D22,D23),AVERAGE(D24,D25),AVERAGE(D26,D17,D17,AVERAGE(D18,D19,D20),AVERAGE(D21,D22,D23),AVERAGE(D24,D25),D17,D17,AVERAGE(D18,D19,D20),AVERAGE(D21,D22,D23),AVERAGE(D24,D25)))</f>
-        <v>-3.1421736023832811</v>
+        <f>AVERAGE(D17,D17,AVERAGE(D18,D19,D20),AVERAGE(D21,D22,D23),AVERAGE(D24,D25),AVERAGE(D26,D17,D17,AVERAGE(D18,D19,D20),AVERAGE(D21,D22,D23),AVERAGE(D24,D25),D17,D17,AVERAGE(D18,D19,D20),AVERAGE(D21,D22,D23),AVERAGE(D24,D25)))</f>
+        <v>-2.6825776427873222</v>
       </c>
       <c r="E28">
-        <f t="shared" si="4"/>
-        <v>1.5362993960518567</v>
+        <f>AVERAGE(E17,E17,AVERAGE(E18,E19,E20),AVERAGE(E21,E22,E23),AVERAGE(E24,E25),AVERAGE(E26,E17,E17,AVERAGE(E18,E19,E20),AVERAGE(E21,E22,E23),AVERAGE(E24,E25),E17,E17,AVERAGE(E18,E19,E20),AVERAGE(E21,E22,E23),AVERAGE(E24,E25)))</f>
+        <v>1.1751882849407453</v>
       </c>
       <c r="F28">
-        <f t="shared" si="4"/>
-        <v>2.5406231858502886</v>
+        <f>AVERAGE(F17,F17,AVERAGE(F18,F19,F20),AVERAGE(F21,F22,F23),AVERAGE(F24,F25),AVERAGE(F26,F17,F17,AVERAGE(F18,F19,F20),AVERAGE(F21,F22,F23),AVERAGE(F24,F25),F17,F17,AVERAGE(F18,F19,F20),AVERAGE(F21,F22,F23),AVERAGE(F24,F25)))</f>
+        <v>1.4466297868603897</v>
       </c>
       <c r="G28">
-        <f t="shared" si="4"/>
-        <v>0.38067987836287737</v>
+        <f>AVERAGE(G17,G17,AVERAGE(G18,G19,G20),AVERAGE(G21,G22,G23),AVERAGE(G24,G25),AVERAGE(G26,G17,G17,AVERAGE(G18,G19,G20),AVERAGE(G21,G22,G23),AVERAGE(G24,G25),G17,G17,AVERAGE(G18,G19,G20),AVERAGE(G21,G22,G23),AVERAGE(G24,G25)))</f>
+        <v>1.3876965803830792</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C29">
         <f>48.22+C28</f>
-        <v>47.563068278794084</v>
+        <v>47.727209692935496</v>
       </c>
       <c r="D29">
         <f>53.14+D28</f>
-        <v>49.99782639761672</v>
+        <v>50.457422357212678</v>
       </c>
       <c r="E29">
         <f>41.56+E28</f>
-        <v>43.096299396051862</v>
+        <v>42.735188284940747</v>
       </c>
       <c r="F29">
         <f>44.45+F28</f>
-        <v>46.990623185850289</v>
+        <v>45.896629786860395</v>
       </c>
       <c r="G29">
         <f>50.71+G28</f>
-        <v>51.090679878362877</v>
+        <v>52.097696580383079</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Integrate observed overall FP votes into live simulations.
</commit_message>
<xml_diff>
--- a/Temporary Region Swings.xlsx
+++ b/Temporary Region Swings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\danny\source\repos\Polling Analyser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djhir\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{043361D8-F416-48A5-B398-16B88CDAAB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06494FD-A61E-453C-B107-A87F2FD01673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16185" yWindow="4845" windowWidth="27960" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12075" yWindow="5730" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="1" r:id="rId1"/>
@@ -487,7 +487,7 @@
   <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26:I27"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,13 +573,13 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J3">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K3">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="L3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M3">
         <v>4</v>
@@ -588,14 +588,14 @@
         <v>3</v>
       </c>
       <c r="O3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P3">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="Q3">
-        <f>K3+L3*0.822+M3*0.348+N3*0.352+(O3+P3)*(0.507)</f>
-        <v>53.067999999999998</v>
+        <f>(K3+L3*0.822+M3*0.348+N3*0.352+(O3+P3)*(0.507))*100/SUM(J3:P3)</f>
+        <v>56.785858585858591</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -629,22 +629,22 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>55</v>
+        <v>51.9</v>
       </c>
       <c r="C5">
-        <v>54</v>
+        <v>52.38</v>
       </c>
       <c r="D5">
-        <v>58</v>
+        <v>53.39</v>
       </c>
       <c r="E5">
-        <v>46</v>
+        <v>46.85</v>
       </c>
       <c r="F5">
-        <v>53</v>
+        <v>51.64</v>
       </c>
       <c r="G5">
-        <v>59</v>
+        <v>53.69</v>
       </c>
       <c r="J5" t="s">
         <v>13</v>
@@ -670,22 +670,22 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>55.5</v>
+        <v>53</v>
       </c>
       <c r="C6">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D6">
-        <v>63.5</v>
+        <v>57</v>
       </c>
       <c r="E6">
-        <v>43.5</v>
+        <v>47</v>
       </c>
       <c r="F6">
+        <v>54.5</v>
+      </c>
+      <c r="G6">
         <v>49</v>
-      </c>
-      <c r="G6">
-        <v>62.5</v>
       </c>
       <c r="J6">
         <v>29.951599999999999</v>
@@ -718,19 +718,19 @@
         <v>54.5</v>
       </c>
       <c r="C7">
-        <v>55</v>
+        <v>51.5</v>
       </c>
       <c r="D7">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E7">
-        <v>45.5</v>
+        <v>46.5</v>
       </c>
       <c r="F7">
-        <v>45.5</v>
+        <v>57.5</v>
       </c>
       <c r="G7">
-        <v>61.5</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -738,22 +738,22 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>55</v>
+        <v>55.5</v>
       </c>
       <c r="C8">
-        <v>53.5</v>
+        <v>56</v>
       </c>
       <c r="D8">
-        <v>58</v>
+        <v>63.5</v>
       </c>
       <c r="E8">
-        <v>51.5</v>
+        <v>43.5</v>
       </c>
       <c r="F8">
         <v>49</v>
       </c>
       <c r="G8">
-        <v>58</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -761,19 +761,19 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>53.885999999999996</v>
+        <v>51.589898989898984</v>
       </c>
       <c r="C9">
-        <v>57.556999999999995</v>
+        <v>47.675510204081633</v>
       </c>
       <c r="D9">
-        <v>53.905000000000001</v>
+        <v>52.043999999999997</v>
       </c>
       <c r="E9">
-        <v>47.676000000000002</v>
+        <v>51.463000000000001</v>
       </c>
       <c r="H9">
-        <v>53.067999999999998</v>
+        <v>56.785858585858591</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -781,19 +781,19 @@
         <v>19</v>
       </c>
       <c r="B10">
-        <v>52.433000000000007</v>
+        <v>53.885999999999996</v>
       </c>
       <c r="C10">
-        <v>52.417999999999992</v>
+        <v>57.556999999999995</v>
       </c>
       <c r="D10">
-        <v>51.266999999999996</v>
+        <v>53.905000000000001</v>
       </c>
       <c r="E10">
-        <v>51.446999999999996</v>
+        <v>47.676000000000002</v>
       </c>
       <c r="H10">
-        <v>53.558999999999997</v>
+        <v>53.067999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -801,19 +801,19 @@
         <v>20</v>
       </c>
       <c r="B11">
-        <v>54.878</v>
+        <v>52.433000000000007</v>
       </c>
       <c r="C11">
-        <v>52.726999999999997</v>
+        <v>52.417999999999992</v>
       </c>
       <c r="D11">
-        <v>53.233999999999995</v>
+        <v>51.266999999999996</v>
       </c>
       <c r="E11">
-        <v>53.542999999999999</v>
+        <v>51.446999999999996</v>
       </c>
       <c r="H11">
-        <v>60.86399999999999</v>
+        <v>53.558999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -917,27 +917,27 @@
       </c>
       <c r="C17">
         <f t="shared" ref="C17:G20" si="0">(C5-C$2)-($B5-$B$2)</f>
-        <v>-0.75</v>
+        <v>0.73000000000000398</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>-1.6700000000000017</v>
+        <v>-3.1799999999999997</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>-2.0900000000000034</v>
+        <v>1.8599999999999994</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>2.019999999999996</v>
+        <v>3.759999999999998</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>1.759999999999998</v>
+        <v>-0.45000000000000284</v>
       </c>
       <c r="H17" s="2">
         <f>F17*0.439183+G17*0.336042</f>
-        <v>1.4785835799999978</v>
+        <v>1.5001091799999982</v>
       </c>
       <c r="J17">
         <v>44.45</v>
@@ -965,27 +965,27 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>-0.75</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>3.3299999999999983</v>
+        <v>-0.67000000000000171</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>-5.0900000000000034</v>
+        <v>0.90999999999999659</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>-2.480000000000004</v>
+        <v>5.519999999999996</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>4.759999999999998</v>
+        <v>-6.240000000000002</v>
       </c>
       <c r="H18" s="2">
         <f>F18*0.439183+G18*0.336042</f>
-        <v>0.51038607999999774</v>
+        <v>0.32738807999999731</v>
       </c>
       <c r="J18">
         <v>1401874</v>
@@ -1009,27 +1009,27 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>-2.75</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>0.82999999999999829</v>
+        <v>1.8299999999999983</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>-2.0900000000000034</v>
+        <v>-1.0900000000000034</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>-4.980000000000004</v>
+        <v>7.019999999999996</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>4.759999999999998</v>
+        <v>5.759999999999998</v>
       </c>
       <c r="H19" s="2">
         <f>F19*0.439183+G19*0.336042</f>
-        <v>-0.5875714200000024</v>
+        <v>5.0186665799999979</v>
       </c>
       <c r="J19">
         <f>J18/SUM($J18:$O18)</f>
@@ -1046,27 +1046,27 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>-1.25</v>
+        <v>0.75</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>-1.6700000000000017</v>
+        <v>3.3299999999999983</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>3.4099999999999966</v>
+        <v>-5.0900000000000034</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>-1.980000000000004</v>
+        <v>-2.480000000000004</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
-        <v>0.75999999999999801</v>
+        <v>4.759999999999998</v>
       </c>
       <c r="H20" s="2">
         <f>F20*0.439183+G20*0.336042</f>
-        <v>-0.61419042000000235</v>
+        <v>0.51038607999999774</v>
       </c>
       <c r="L20">
         <f>(J18+K18)/SUM(J18:O18)</f>
@@ -1079,27 +1079,27 @@
       </c>
       <c r="C21">
         <f t="shared" ref="C21:E26" si="1">(C9-C$2)-($B9-$B$2)</f>
-        <v>3.9209999999999994</v>
+        <v>-3.6643887858173514</v>
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
-        <v>-4.6509999999999962</v>
+        <v>-4.2158989898989887</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
-        <v>0.70000000000000284</v>
+        <v>6.7831010101010136</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" ref="F21:G23" si="2">AVERAGE(F$17,F$17,F$17,F$17,F$17,F$17,F$18,F$19,F$20)+($H21-AVERAGE($H$17,$H$17,$H$17,$H$17,$H$17,$H$17,$H$18,$H$19,$H$20))</f>
-        <v>-2.5136238796580139</v>
+        <v>6.0851168163015918</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="2"/>
-        <v>-0.49584610188023426</v>
+        <v>2.636227927412703</v>
       </c>
       <c r="H21">
         <f>(H9-H$2)-($B9-$B$2)</f>
-        <v>-1.9024987996580123</v>
+        <v>4.1114607963015928</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -1108,27 +1108,27 @@
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>0.23499999999998522</v>
+        <v>3.9209999999999994</v>
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
-        <v>-5.8360000000000127</v>
+        <v>-4.6509999999999962</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
-        <v>5.9239999999999853</v>
+        <v>0.70000000000000284</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="2"/>
-        <v>-0.56962387965802563</v>
+        <v>7.1157220341986793E-2</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="2"/>
-        <v>1.4481538981197539</v>
+        <v>-3.3777316685469021</v>
       </c>
       <c r="H22">
         <f>(H10-H$2)-($B10-$B$2)</f>
-        <v>4.150120034197613E-2</v>
+        <v>-1.9024987996580123</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -1137,27 +1137,27 @@
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>-1.9010000000000034</v>
+        <v>0.23499999999998522</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>-6.3140000000000072</v>
+        <v>-5.8360000000000127</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
-        <v>5.5749999999999957</v>
+        <v>5.9239999999999853</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="2"/>
-        <v>4.2903761203419739</v>
+        <v>2.0151572203419752</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="2"/>
-        <v>6.3081538981197536</v>
+        <v>-1.4337316685469133</v>
       </c>
       <c r="H23">
         <f>(H11-H$2)-($B11-$B$2)</f>
-        <v>4.9015012003419756</v>
+        <v>4.150120034197613E-2</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -1250,45 +1250,45 @@
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C28">
         <f>AVERAGE(C17,C17,AVERAGE(C18,C19,C20),AVERAGE(C21,C22,C23),AVERAGE(C24,C25),AVERAGE(C26,C17,C17,AVERAGE(C18,C19,C20),AVERAGE(C21,C22,C23),AVERAGE(C24,C25),C17,C17,AVERAGE(C18,C19,C20),AVERAGE(C21,C22,C23),AVERAGE(C24,C25)))</f>
-        <v>-0.49279030706450122</v>
+        <v>-0.22250775259796188</v>
       </c>
       <c r="D28">
         <f>AVERAGE(D17,D17,AVERAGE(D18,D19,D20),AVERAGE(D21,D22,D23),AVERAGE(D24,D25),AVERAGE(D26,D17,D17,AVERAGE(D18,D19,D20),AVERAGE(D21,D22,D23),AVERAGE(D24,D25),D17,D17,AVERAGE(D18,D19,D20),AVERAGE(D21,D22,D23),AVERAGE(D24,D25)))</f>
-        <v>-2.6825776427873222</v>
+        <v>-3.0083588895988704</v>
       </c>
       <c r="E28">
         <f>AVERAGE(E17,E17,AVERAGE(E18,E19,E20),AVERAGE(E21,E22,E23),AVERAGE(E24,E25),AVERAGE(E26,E17,E17,AVERAGE(E18,E19,E20),AVERAGE(E21,E22,E23),AVERAGE(E24,E25),E17,E17,AVERAGE(E18,E19,E20),AVERAGE(E21,E22,E23),AVERAGE(E24,E25)))</f>
-        <v>1.1751882849407453</v>
+        <v>2.7120838058059644</v>
       </c>
       <c r="F28">
         <f>AVERAGE(F17,F17,AVERAGE(F18,F19,F20),AVERAGE(F21,F22,F23),AVERAGE(F24,F25),AVERAGE(F26,F17,F17,AVERAGE(F18,F19,F20),AVERAGE(F21,F22,F23),AVERAGE(F24,F25),F17,F17,AVERAGE(F18,F19,F20),AVERAGE(F21,F22,F23),AVERAGE(F24,F25)))</f>
-        <v>1.4466297868603897</v>
+        <v>3.8696395729587487</v>
       </c>
       <c r="G28">
         <f>AVERAGE(G17,G17,AVERAGE(G18,G19,G20),AVERAGE(G21,G22,G23),AVERAGE(G24,G25),AVERAGE(G26,G17,G17,AVERAGE(G18,G19,G20),AVERAGE(G21,G22,G23),AVERAGE(G24,G25),G17,G17,AVERAGE(G18,G19,G20),AVERAGE(G21,G22,G23),AVERAGE(G24,G25)))</f>
-        <v>1.3876965803830792</v>
+        <v>-0.49636434058926943</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C29">
         <f>48.22+C28</f>
-        <v>47.727209692935496</v>
+        <v>47.997492247402036</v>
       </c>
       <c r="D29">
         <f>53.14+D28</f>
-        <v>50.457422357212678</v>
+        <v>50.131641110401134</v>
       </c>
       <c r="E29">
         <f>41.56+E28</f>
-        <v>42.735188284940747</v>
+        <v>44.27208380580597</v>
       </c>
       <c r="F29">
         <f>44.45+F28</f>
-        <v>45.896629786860395</v>
+        <v>48.319639572958749</v>
       </c>
       <c r="G29">
         <f>50.71+G28</f>
-        <v>52.097696580383079</v>
+        <v>50.213635659410734</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>